<commit_message>
feature/tests: update test-cases-15-15.xlsx and add test-case-files bulk deserialization tes
</commit_message>
<xml_diff>
--- a/csv_parser/test-cases-15-15.xlsx
+++ b/csv_parser/test-cases-15-15.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/13 - 15-15/04 - Pilotes 15-15/04 - JDD recette/JSON pour interface LRM/03 - Automodel tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86598866-B0CA-483B-BEF4-746274D73198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EC48BF3-E648-457F-A3F9-F3C403454E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3285" yWindow="1590" windowWidth="22740" windowHeight="12930" xr2:uid="{8E95E427-60E8-4C01-A0F5-EF6B52DBDF48}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Partage de dossier simple" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Partage de dossier simple'!$A$9:$P$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Partage de dossier simple'!$A$9:$O$88</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +44,7 @@
     <author>tc={FB75C0C9-7A43-4C0C-BF65-EEEEE383A568}</author>
   </authors>
   <commentList>
-    <comment ref="G65" authorId="0" shapeId="0" xr:uid="{FB75C0C9-7A43-4C0C-BF65-EEEEE383A568}">
+    <comment ref="F65" authorId="0" shapeId="0" xr:uid="{FB75C0C9-7A43-4C0C-BF65-EEEEE383A568}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="285">
   <si>
     <t>Périmètre</t>
   </si>
@@ -117,9 +117,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Donnée</t>
   </si>
   <si>
@@ -631,9 +628,6 @@
   </si>
   <si>
     <t>2024-01-04T00:05:00+01:00</t>
-  </si>
-  <si>
-    <t>number</t>
   </si>
   <si>
     <t>Géométrie Associée / Point / Latitude</t>
@@ -925,7 +919,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1034,18 +1028,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1634,7 +1616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1670,22 +1652,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1699,28 +1666,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1749,9 +1695,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1782,9 +1725,6 @@
     <xf numFmtId="49" fontId="12" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1796,18 +1736,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1848,9 +1782,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1864,9 +1795,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1875,9 +1803,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1891,9 +1816,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1940,9 +1862,6 @@
     </xf>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1951,9 +1870,6 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2007,101 +1923,59 @@
     <xf numFmtId="49" fontId="12" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF58383"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF58383"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <fill>
         <patternFill>
@@ -2655,7 +2529,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G65" dT="2023-09-22T09:00:43.88" personId="{EC126A12-45AA-40A1-AD6A-8686E0786064}" id="{FB75C0C9-7A43-4C0C-BF65-EEEEE383A568}" done="1">
+  <threadedComment ref="F65" dT="2023-09-22T09:00:43.88" personId="{EC126A12-45AA-40A1-AD6A-8686E0786064}" id="{FB75C0C9-7A43-4C0C-BF65-EEEEE383A568}" done="1">
     <text>Pour savoir quelle alerte utiliser dans une affaire :
 =&gt; Regarder cette date de réception</text>
   </threadedComment>
@@ -2664,11 +2538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC96D3DE-56F6-4E60-B012-339ED5333B2B}">
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="7" ySplit="10" topLeftCell="H67" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I77" sqref="I77"/>
+      <pane xSplit="6" ySplit="10" topLeftCell="G37" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F1048576"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
     </sheetView>
@@ -2680,796 +2554,767 @@
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="3.140625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="47.140625" customWidth="1"/>
-    <col min="8" max="8" width="63.28515625" customWidth="1"/>
-    <col min="9" max="9" width="48.140625" style="3" customWidth="1"/>
-    <col min="10" max="11" width="48.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" customWidth="1"/>
+    <col min="7" max="7" width="63.28515625" customWidth="1"/>
+    <col min="8" max="8" width="48.140625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="48.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:15" ht="18.75">
+      <c r="A1" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="160"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="27"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="18.75">
-      <c r="A2" s="24" t="s">
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A2" s="160" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="160"/>
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="J2" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-    </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="18.75">
-      <c r="A3" s="24" t="s">
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A3" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="160"/>
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-    </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="18.75">
-      <c r="A4" s="24" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
+      <c r="L3" s="159"/>
+      <c r="M3" s="159"/>
+      <c r="N3" s="159"/>
+      <c r="O3" s="159"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A4" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="160"/>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-    </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="18.75">
-      <c r="A5" s="32" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="159"/>
+      <c r="K4" s="159"/>
+      <c r="L4" s="159"/>
+      <c r="M4" s="159"/>
+      <c r="N4" s="159"/>
+      <c r="O4" s="159"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A5" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-    </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="18.75">
-      <c r="A6" s="34" t="s">
+      <c r="B5" s="171"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A6" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="6" t="s">
+      <c r="B6" s="162"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-    </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="37" t="s">
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A7" s="172" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="6" t="s">
+      <c r="B7" s="172"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-    </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="18.75">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="6" t="s">
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-    </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" ht="18.75">
-      <c r="A9" s="41" t="s">
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+    </row>
+    <row r="9" spans="1:15" s="2" customFormat="1" ht="18.75">
+      <c r="A9" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="46" t="s">
+      <c r="J9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="46" t="s">
+      <c r="K9" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="46" t="s">
+      <c r="L9" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="46" t="s">
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="48" t="s">
+      <c r="B10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="C10" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="D10" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="50" t="s">
-        <v>30</v>
-      </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" ht="16.5" customHeight="1">
+    </row>
+    <row r="11" spans="1:15" ht="16.5" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="173" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="56" t="s">
+      <c r="G11" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="57" t="s">
+      <c r="H11" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="58" t="s">
+      <c r="I11" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:16">
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="60" t="s">
+      <c r="D12" s="173"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="61" t="s">
+      <c r="H12" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="K12" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="63"/>
-      <c r="M12" s="63"/>
+      <c r="I12" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:16">
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="64" t="s">
+      <c r="D13" s="173"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="58" t="s">
+      <c r="H13" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="I13" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
+      <c r="J13" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" s="4" customFormat="1">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="54"/>
+    </row>
+    <row r="14" spans="1:15" s="4" customFormat="1">
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="173"/>
       <c r="E14" s="17">
         <v>3</v>
       </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="66" t="s">
+      <c r="F14" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="67" t="s">
+      <c r="H14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="68" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" s="68" t="s">
-        <v>46</v>
-      </c>
-      <c r="K14" s="68" t="s">
-        <v>46</v>
-      </c>
-      <c r="L14" s="67"/>
-      <c r="M14" s="67"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="65"/>
-      <c r="P14" s="65"/>
-    </row>
-    <row r="15" spans="1:16" s="4" customFormat="1">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="54"/>
+      <c r="I14" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+    </row>
+    <row r="15" spans="1:15" s="4" customFormat="1">
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="173"/>
       <c r="E15" s="17">
         <v>3</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="66" t="s">
+      <c r="F15" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="67" t="s">
+      <c r="H15" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="K15" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="65"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="I15" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="69" t="s">
+      <c r="D16" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="70"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="72" t="s">
+      <c r="G16" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="73" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="74"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="1:16">
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="70"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="74"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="1:16">
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="77" t="s">
+      <c r="D18" s="164" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="42">
+        <v>2</v>
+      </c>
+      <c r="F18" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="55">
-        <v>2</v>
-      </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="78" t="s">
+      <c r="G18" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="79" t="s">
+      <c r="H18" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="I18" s="80" t="s">
+      <c r="I18" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="80" t="s">
+      <c r="J18" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="K18" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:16" ht="28.5" customHeight="1">
+    </row>
+    <row r="19" spans="1:15" ht="28.5" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="55">
+      <c r="D19" s="165"/>
+      <c r="E19" s="42">
         <v>3</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="83" t="s">
+      <c r="F19" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="84" t="s">
+      <c r="H19" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="I19" s="85" t="s">
+      <c r="I19" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="85" t="s">
+      <c r="J19" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="86" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="1:16">
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="82"/>
+      <c r="D20" s="165"/>
       <c r="E20" s="17">
         <v>2</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="88" t="s">
+      <c r="F20" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="89" t="s">
+      <c r="H20" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="90" t="s">
+      <c r="I20" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="J20" s="89" t="s">
+      <c r="J20" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="K20" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="89"/>
-      <c r="M20" s="89"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" s="8" customFormat="1" ht="30.75">
-      <c r="A21" s="91"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="92">
+    </row>
+    <row r="21" spans="1:15" s="8" customFormat="1" ht="30.75">
+      <c r="A21" s="75"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="165"/>
+      <c r="E21" s="76">
         <v>3</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="93" t="s">
+      <c r="F21" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="H21" s="49" t="s">
+      <c r="H21" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="I21" s="94" t="s">
+      <c r="I21" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="J21" s="94" t="s">
+      <c r="J21" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="K21" s="95" t="s">
-        <v>75</v>
-      </c>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="91"/>
-      <c r="O21" s="91"/>
-      <c r="P21" s="91"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="75"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="75"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="82"/>
+      <c r="D22" s="165"/>
       <c r="E22" s="17">
         <v>1</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="96" t="s">
+      <c r="F22" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="97" t="s">
+      <c r="H22" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="I22" s="98" t="s">
+      <c r="I22" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="J22" s="97" t="s">
+      <c r="J22" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="K22" s="97" t="s">
-        <v>80</v>
-      </c>
-      <c r="L22" s="97"/>
-      <c r="M22" s="97"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="1:16" ht="30.75" customHeight="1">
+    </row>
+    <row r="23" spans="1:15" ht="30.75" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="82"/>
-      <c r="E23" s="92">
+      <c r="D23" s="165"/>
+      <c r="E23" s="76">
         <v>3</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="13" t="s">
+      <c r="F23" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="I23" s="99" t="s">
+      <c r="I23" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="J23" s="100" t="s">
+      <c r="J23" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="K23" s="100" t="s">
-        <v>85</v>
-      </c>
+      <c r="K23" s="5"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-    </row>
-    <row r="24" spans="1:16">
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="82"/>
+      <c r="D24" s="165"/>
       <c r="E24" s="17">
         <v>1</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="13" t="s">
+      <c r="F24" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="I24" s="99" t="s">
+      <c r="I24" s="5" t="s">
         <v>88</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="K24" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="K24" s="5"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-    </row>
-    <row r="25" spans="1:16">
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="102">
+      <c r="D25" s="166"/>
+      <c r="E25" s="85">
         <v>3</v>
       </c>
-      <c r="F25" s="71"/>
-      <c r="G25" s="103" t="s">
+      <c r="F25" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="75" t="s">
+      <c r="H25" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="J25" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="K25" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="L25" s="75"/>
-      <c r="M25" s="75"/>
+      <c r="I25" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-    </row>
-    <row r="26" spans="1:16">
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="104" t="s">
+      <c r="D26" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="42">
+        <v>1</v>
+      </c>
+      <c r="F26" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" s="89" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="55">
-        <v>1</v>
-      </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="105" t="s">
-        <v>94</v>
-      </c>
-      <c r="H26" s="106" t="s">
+      <c r="H26" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="I26" s="107" t="s">
+      <c r="I26" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="J26" s="107" t="s">
+      <c r="J26" s="90" t="s">
         <v>97</v>
       </c>
-      <c r="K26" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="L26" s="108"/>
-      <c r="M26" s="108"/>
+      <c r="K26" s="91"/>
+      <c r="L26" s="91"/>
+      <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-    </row>
-    <row r="27" spans="1:16">
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="109" t="s">
+      <c r="D27" s="168" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="92"/>
+      <c r="F27" s="93" t="s">
         <v>99</v>
       </c>
-      <c r="E27" s="110"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="111" t="s">
+      <c r="G27" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="H27" s="112" t="s">
+      <c r="H27" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="I27" s="113" t="s">
+      <c r="I27" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="J27" s="113" t="s">
+      <c r="J27" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="K27" s="113" t="s">
-        <v>104</v>
-      </c>
+      <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
+      <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-    </row>
-    <row r="28" spans="1:16">
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="114"/>
+      <c r="D28" s="169"/>
       <c r="E28" s="17">
         <v>1</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="13" t="s">
+      <c r="F28" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="I28" s="99" t="s">
+      <c r="I28" s="5" t="s">
         <v>107</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="K28" s="5" t="s">
-        <v>109</v>
-      </c>
+      <c r="K28" s="5"/>
       <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
+      <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-    </row>
-    <row r="29" spans="1:16" s="6" customFormat="1">
-      <c r="D29" s="114"/>
+    </row>
+    <row r="29" spans="1:15" s="6" customFormat="1">
+      <c r="D29" s="169"/>
       <c r="E29" s="17">
         <v>2</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="13" t="s">
+      <c r="F29" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>110</v>
       </c>
       <c r="H29" s="5" t="s">
@@ -3478,1713 +3323,1601 @@
       <c r="I29" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="J29" s="5" t="s">
-        <v>113</v>
-      </c>
+      <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-    </row>
-    <row r="30" spans="1:16">
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="114"/>
+      <c r="D30" s="169"/>
       <c r="E30" s="17">
         <v>1</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="13" t="s">
+      <c r="F30" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="83" t="s">
         <v>115</v>
       </c>
-      <c r="I30" s="99" t="s">
+      <c r="I30" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J30" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
+      <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-    </row>
-    <row r="31" spans="1:16">
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="114"/>
+      <c r="D31" s="169"/>
       <c r="E31" s="17"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="13" t="s">
+      <c r="F31" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="I31" s="99" t="s">
+      <c r="I31" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="J31" s="5" t="s">
-        <v>121</v>
-      </c>
+      <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
+      <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-    </row>
-    <row r="32" spans="1:16">
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="114"/>
+      <c r="D32" s="169"/>
       <c r="E32" s="17"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="13" t="s">
+      <c r="F32" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="I32" s="99" t="s">
+      <c r="I32" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="J32" s="5" t="s">
-        <v>125</v>
-      </c>
+      <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
+      <c r="M32" s="6"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-    </row>
-    <row r="33" spans="1:16" s="4" customFormat="1">
-      <c r="A33" s="65"/>
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="114"/>
+    </row>
+    <row r="33" spans="1:15" s="4" customFormat="1">
+      <c r="A33" s="52"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="169"/>
       <c r="E33" s="17">
         <v>2</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="115" t="s">
+      <c r="F33" s="96" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="H33" s="116" t="s">
+      <c r="H33" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="I33" s="117" t="s">
+      <c r="I33" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="J33" s="118" t="s">
+      <c r="J33" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="K33" s="118" t="s">
-        <v>130</v>
-      </c>
-      <c r="L33" s="118"/>
-      <c r="M33" s="118"/>
-      <c r="N33" s="65"/>
-      <c r="O33" s="65"/>
-      <c r="P33" s="65"/>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="K33" s="99"/>
+      <c r="L33" s="99"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="52"/>
+      <c r="O33" s="52"/>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="109" t="s">
+      <c r="D34" s="168" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="92"/>
+      <c r="F34" s="100" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="110"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="119" t="s">
-        <v>100</v>
-      </c>
-      <c r="H34" s="112" t="s">
-        <v>132</v>
-      </c>
-      <c r="I34" s="120"/>
-      <c r="J34" s="120"/>
-      <c r="K34" s="121"/>
-      <c r="L34" s="121"/>
-      <c r="M34" s="122"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="102"/>
+      <c r="K34" s="102"/>
+      <c r="L34" s="103"/>
+      <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-    </row>
-    <row r="35" spans="1:16">
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="114"/>
+      <c r="D35" s="169"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I35" s="99"/>
+      <c r="F35" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H35" s="83"/>
+      <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="123"/>
+      <c r="L35" s="104"/>
+      <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-    </row>
-    <row r="36" spans="1:16">
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="114"/>
+      <c r="D36" s="169"/>
       <c r="E36" s="17"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="I36" s="99"/>
+      <c r="F36" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H36" s="83"/>
+      <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="123"/>
+      <c r="L36" s="104"/>
+      <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-    </row>
-    <row r="37" spans="1:16">
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="114"/>
+      <c r="D37" s="169"/>
       <c r="E37" s="17"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="I37" s="99"/>
+      <c r="F37" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H37" s="83"/>
+      <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="123"/>
+      <c r="L37" s="104"/>
+      <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-    </row>
-    <row r="38" spans="1:16">
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="114"/>
+      <c r="D38" s="169"/>
       <c r="E38" s="17"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I38" s="99"/>
+      <c r="F38" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H38" s="83"/>
+      <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="123"/>
+      <c r="L38" s="104"/>
+      <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-    </row>
-    <row r="39" spans="1:16">
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="114"/>
+      <c r="D39" s="169"/>
       <c r="E39" s="17"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="I39" s="99"/>
+      <c r="F39" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H39" s="83"/>
+      <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="123"/>
+      <c r="L39" s="104"/>
+      <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-    </row>
-    <row r="40" spans="1:16">
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
-      <c r="D40" s="124"/>
+      <c r="D40" s="170"/>
       <c r="E40" s="17"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="125" t="s">
-        <v>126</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="I40" s="126"/>
-      <c r="J40" s="127"/>
-      <c r="K40" s="127"/>
-      <c r="L40" s="127"/>
-      <c r="M40" s="128"/>
+      <c r="F40" s="105" t="s">
+        <v>125</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H40" s="106"/>
+      <c r="I40" s="107"/>
+      <c r="J40" s="107"/>
+      <c r="K40" s="107"/>
+      <c r="L40" s="108"/>
+      <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-    </row>
-    <row r="41" spans="1:16">
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="77" t="s">
+      <c r="D41" s="164" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41" s="42"/>
+      <c r="F41" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="E41" s="55"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="129" t="s">
+      <c r="G41" s="89" t="s">
         <v>140</v>
       </c>
-      <c r="H41" s="106" t="s">
+      <c r="H41" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="I41" s="107" t="s">
+      <c r="I41" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="J41" s="107" t="s">
+      <c r="J41" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="K41" s="107" t="s">
-        <v>144</v>
-      </c>
-      <c r="L41" s="108"/>
-      <c r="M41" s="108"/>
+      <c r="K41" s="91"/>
+      <c r="L41" s="91"/>
+      <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-    </row>
-    <row r="42" spans="1:16">
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
-      <c r="D42" s="82"/>
+      <c r="D42" s="165"/>
       <c r="E42" s="17">
         <v>2</v>
       </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="130" t="s">
+      <c r="F42" s="110" t="s">
+        <v>144</v>
+      </c>
+      <c r="G42" s="111" t="s">
         <v>145</v>
       </c>
-      <c r="H42" s="131" t="s">
+      <c r="H42" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="I42" s="132" t="s">
-        <v>147</v>
-      </c>
-      <c r="J42" s="132" t="s">
-        <v>147</v>
-      </c>
-      <c r="K42" s="132" t="s">
-        <v>147</v>
-      </c>
-      <c r="L42" s="133"/>
-      <c r="M42" s="133"/>
+      <c r="I42" s="112" t="s">
+        <v>146</v>
+      </c>
+      <c r="J42" s="112" t="s">
+        <v>146</v>
+      </c>
+      <c r="K42" s="113"/>
+      <c r="L42" s="113"/>
+      <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-    </row>
-    <row r="43" spans="1:16" s="4" customFormat="1">
-      <c r="A43" s="65"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="82"/>
+    </row>
+    <row r="43" spans="1:15" s="4" customFormat="1">
+      <c r="A43" s="52"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="165"/>
       <c r="E43" s="17"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="134" t="s">
+      <c r="F43" s="114" t="s">
+        <v>147</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="H43" s="115"/>
+      <c r="I43" s="115"/>
+      <c r="J43" s="115" t="s">
         <v>149</v>
       </c>
-      <c r="I43" s="135"/>
-      <c r="J43" s="135"/>
-      <c r="K43" s="135" t="s">
-        <v>150</v>
-      </c>
-      <c r="L43" s="136"/>
-      <c r="M43" s="136"/>
-      <c r="N43" s="65"/>
-      <c r="O43" s="65"/>
-      <c r="P43" s="65"/>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="K43" s="116"/>
+      <c r="L43" s="116"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="52"/>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="110">
+      <c r="D44" s="165"/>
+      <c r="E44" s="92">
         <v>1</v>
       </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="137" t="s">
+      <c r="F44" s="117" t="s">
+        <v>150</v>
+      </c>
+      <c r="G44" s="118" t="s">
         <v>151</v>
       </c>
-      <c r="H44" s="138" t="s">
+      <c r="H44" s="119" t="s">
         <v>152</v>
       </c>
-      <c r="I44" s="139" t="s">
+      <c r="I44" s="119" t="s">
         <v>153</v>
       </c>
-      <c r="J44" s="139" t="s">
+      <c r="J44" s="120" t="s">
         <v>154</v>
       </c>
-      <c r="K44" s="140" t="s">
-        <v>155</v>
-      </c>
-      <c r="L44" s="140"/>
-      <c r="M44" s="140"/>
+      <c r="K44" s="120"/>
+      <c r="L44" s="120"/>
+      <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-    </row>
-    <row r="45" spans="1:16">
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
-      <c r="D45" s="82"/>
+      <c r="D45" s="165"/>
       <c r="E45" s="17">
         <v>1</v>
       </c>
-      <c r="F45" s="22"/>
-      <c r="G45" s="13" t="s">
+      <c r="F45" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="I45" s="99" t="s">
+      <c r="I45" s="5" t="s">
         <v>158</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="K45" s="5" t="s">
-        <v>160</v>
-      </c>
+      <c r="K45" s="5"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
+      <c r="M45" s="6"/>
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-    </row>
-    <row r="46" spans="1:16">
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="82"/>
+      <c r="D46" s="165"/>
       <c r="E46" s="17">
         <v>3</v>
       </c>
-      <c r="F46" s="22"/>
-      <c r="G46" s="13" t="s">
+      <c r="F46" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H46" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="I46" s="141">
+      <c r="H46" s="121">
         <v>77479</v>
       </c>
-      <c r="J46" s="141">
+      <c r="I46" s="121">
         <v>95063</v>
       </c>
-      <c r="K46" s="141">
+      <c r="J46" s="121">
         <v>9029</v>
       </c>
-      <c r="L46" s="141"/>
-      <c r="M46" s="141"/>
+      <c r="K46" s="121"/>
+      <c r="L46" s="121"/>
+      <c r="M46" s="6"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-    </row>
-    <row r="47" spans="1:16">
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
-      <c r="D47" s="82"/>
+      <c r="D47" s="165"/>
       <c r="E47" s="17">
         <v>2</v>
       </c>
-      <c r="F47" s="22"/>
-      <c r="G47" s="13" t="s">
+      <c r="F47" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="H47" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="I47" s="5"/>
-      <c r="J47" s="142">
+      <c r="H47" s="5"/>
+      <c r="I47" s="122">
         <v>3</v>
       </c>
+      <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
+      <c r="M47" s="6"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
-      <c r="P47" s="6"/>
-    </row>
-    <row r="48" spans="1:16">
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
-      <c r="D48" s="82"/>
+      <c r="D48" s="165"/>
       <c r="E48" s="17">
         <v>2</v>
       </c>
-      <c r="F48" s="22"/>
-      <c r="G48" s="13" t="s">
+      <c r="F48" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="H48" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="I48" s="5"/>
-      <c r="J48" s="6"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="5"/>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
+      <c r="M48" s="6"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
-      <c r="P48" s="6"/>
-    </row>
-    <row r="49" spans="1:16">
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="82"/>
+      <c r="D49" s="165"/>
       <c r="E49" s="17">
         <v>2</v>
       </c>
-      <c r="F49" s="22"/>
-      <c r="G49" s="13" t="s">
+      <c r="F49" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5" t="s">
-        <v>125</v>
-      </c>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
+      <c r="M49" s="6"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
-    </row>
-    <row r="50" spans="1:16">
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
-      <c r="D50" s="82"/>
+      <c r="D50" s="165"/>
       <c r="E50" s="17">
         <v>2</v>
       </c>
-      <c r="F50" s="22"/>
-      <c r="G50" s="13" t="s">
+      <c r="F50" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="I50" s="5"/>
-      <c r="J50" s="143">
+      <c r="H50" s="5"/>
+      <c r="I50" s="123">
         <v>5678</v>
       </c>
+      <c r="J50" s="5"/>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
+      <c r="M50" s="6"/>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
-      <c r="P50" s="6"/>
-    </row>
-    <row r="51" spans="1:16">
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
-      <c r="D51" s="82"/>
+      <c r="D51" s="165"/>
       <c r="E51" s="17">
         <v>2</v>
       </c>
-      <c r="F51" s="22"/>
-      <c r="G51" s="13" t="s">
+      <c r="F51" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="H51" s="5"/>
+      <c r="I51" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5" t="s">
-        <v>173</v>
-      </c>
+      <c r="J51" s="5"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
+      <c r="M51" s="6"/>
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-    </row>
-    <row r="52" spans="1:16">
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
-      <c r="D52" s="82"/>
+      <c r="D52" s="165"/>
       <c r="E52" s="17">
         <v>2</v>
       </c>
-      <c r="F52" s="22"/>
-      <c r="G52" s="13" t="s">
+      <c r="F52" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H52" s="5"/>
+      <c r="I52" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5" t="s">
-        <v>176</v>
-      </c>
+      <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
+      <c r="M52" s="6"/>
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-    </row>
-    <row r="53" spans="1:16">
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
-      <c r="D53" s="82"/>
+      <c r="D53" s="165"/>
       <c r="E53" s="17">
         <v>2</v>
       </c>
-      <c r="F53" s="22"/>
-      <c r="G53" s="13" t="s">
+      <c r="F53" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="H53" s="5" t="s">
-        <v>178</v>
-      </c>
+      <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
+      <c r="M53" s="6"/>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-    </row>
-    <row r="54" spans="1:16">
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
-      <c r="D54" s="82"/>
+      <c r="D54" s="165"/>
       <c r="E54" s="17">
         <v>2</v>
       </c>
-      <c r="F54" s="22"/>
-      <c r="G54" s="13" t="s">
+      <c r="F54" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>180</v>
-      </c>
+      <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
+      <c r="M54" s="6"/>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
-    </row>
-    <row r="55" spans="1:16">
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
-      <c r="D55" s="82"/>
+      <c r="D55" s="165"/>
       <c r="E55" s="17">
         <v>2</v>
       </c>
-      <c r="F55" s="22"/>
-      <c r="G55" s="144" t="s">
+      <c r="F55" s="124" t="s">
+        <v>180</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="H55" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I55" s="145"/>
-      <c r="J55" s="145"/>
-      <c r="K55" s="143">
+      <c r="H55" s="125"/>
+      <c r="I55" s="125"/>
+      <c r="J55" s="123">
         <v>561964589</v>
       </c>
+      <c r="K55" s="5"/>
       <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
+      <c r="M55" s="6"/>
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-    </row>
-    <row r="56" spans="1:16" s="4" customFormat="1">
-      <c r="A56" s="65"/>
-      <c r="B56" s="65"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="82"/>
+    </row>
+    <row r="56" spans="1:15" s="4" customFormat="1">
+      <c r="A56" s="52"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="165"/>
       <c r="E56" s="17">
         <v>2</v>
       </c>
-      <c r="F56" s="22"/>
-      <c r="G56" s="66" t="s">
+      <c r="F56" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H56" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="I56" s="67" t="s">
+      <c r="I56" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="J56" s="67" t="s">
+      <c r="J56" s="126" t="s">
         <v>186</v>
       </c>
-      <c r="K56" s="146" t="s">
-        <v>187</v>
-      </c>
-      <c r="L56" s="116"/>
-      <c r="M56" s="116"/>
-      <c r="N56" s="65"/>
-      <c r="O56" s="65"/>
-      <c r="P56" s="65"/>
-    </row>
-    <row r="57" spans="1:16">
+      <c r="K56" s="97"/>
+      <c r="L56" s="97"/>
+      <c r="M56" s="52"/>
+      <c r="N56" s="52"/>
+      <c r="O56" s="52"/>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="110"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="147" t="s">
+      <c r="D57" s="165"/>
+      <c r="E57" s="92"/>
+      <c r="F57" s="127" t="s">
+        <v>187</v>
+      </c>
+      <c r="G57" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="H57" s="148" t="s">
+      <c r="H57" s="128" t="s">
         <v>189</v>
       </c>
-      <c r="I57" s="148" t="s">
-        <v>190</v>
-      </c>
-      <c r="J57" s="149" t="s">
-        <v>190</v>
-      </c>
-      <c r="K57" s="148"/>
-      <c r="L57" s="97"/>
-      <c r="M57" s="97"/>
+      <c r="I57" s="129" t="s">
+        <v>189</v>
+      </c>
+      <c r="J57" s="128"/>
+      <c r="K57" s="81"/>
+      <c r="L57" s="81"/>
+      <c r="M57" s="6"/>
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
-      <c r="P57" s="6"/>
-    </row>
-    <row r="58" spans="1:16">
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="110">
+      <c r="D58" s="165"/>
+      <c r="E58" s="92">
         <v>3</v>
       </c>
-      <c r="F58" s="150" t="s">
+      <c r="F58" s="130" t="s">
+        <v>190</v>
+      </c>
+      <c r="G58" s="128" t="s">
         <v>191</v>
       </c>
-      <c r="G58" s="151" t="s">
+      <c r="H58" s="131" t="s">
         <v>192</v>
       </c>
-      <c r="H58" s="148" t="s">
+      <c r="I58" s="132" t="s">
         <v>193</v>
       </c>
-      <c r="I58" s="152" t="s">
-        <v>194</v>
-      </c>
-      <c r="J58" s="153" t="s">
-        <v>195</v>
-      </c>
-      <c r="K58" s="152"/>
-      <c r="L58" s="97"/>
-      <c r="M58" s="97"/>
+      <c r="J58" s="131"/>
+      <c r="K58" s="81"/>
+      <c r="L58" s="81"/>
+      <c r="M58" s="6"/>
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
-      <c r="P58" s="6"/>
-    </row>
-    <row r="59" spans="1:16">
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
-      <c r="D59" s="82"/>
-      <c r="E59" s="110">
+      <c r="D59" s="165"/>
+      <c r="E59" s="92">
         <v>3</v>
       </c>
-      <c r="F59" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G59" s="151" t="s">
+      <c r="F59" s="130" t="s">
+        <v>194</v>
+      </c>
+      <c r="G59" s="128" t="s">
+        <v>195</v>
+      </c>
+      <c r="H59" s="131" t="s">
         <v>196</v>
       </c>
-      <c r="H59" s="148" t="s">
+      <c r="I59" s="132" t="s">
         <v>197</v>
       </c>
-      <c r="I59" s="152" t="s">
-        <v>198</v>
-      </c>
-      <c r="J59" s="153" t="s">
-        <v>199</v>
-      </c>
-      <c r="K59" s="152"/>
-      <c r="L59" s="97"/>
-      <c r="M59" s="97"/>
+      <c r="J59" s="131"/>
+      <c r="K59" s="81"/>
+      <c r="L59" s="81"/>
+      <c r="M59" s="6"/>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
-      <c r="P59" s="6"/>
-    </row>
-    <row r="60" spans="1:16">
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
-      <c r="D60" s="82"/>
+      <c r="D60" s="165"/>
       <c r="E60" s="17"/>
-      <c r="F60" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G60" s="154" t="s">
-        <v>200</v>
-      </c>
-      <c r="H60" s="140" t="s">
-        <v>201</v>
-      </c>
-      <c r="I60" s="140"/>
+      <c r="F60" s="133" t="s">
+        <v>198</v>
+      </c>
+      <c r="G60" s="120" t="s">
+        <v>199</v>
+      </c>
+      <c r="H60" s="120"/>
+      <c r="I60" s="5"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
+      <c r="M60" s="6"/>
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
-      <c r="P60" s="6"/>
-    </row>
-    <row r="61" spans="1:16">
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
-      <c r="D61" s="82"/>
+      <c r="D61" s="165"/>
       <c r="E61" s="17"/>
-      <c r="F61" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H61" s="140" t="s">
-        <v>203</v>
-      </c>
+      <c r="F61" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G61" s="120" t="s">
+        <v>201</v>
+      </c>
+      <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
+      <c r="M61" s="6"/>
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
-      <c r="P61" s="6"/>
-    </row>
-    <row r="62" spans="1:16">
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
-      <c r="D62" s="82"/>
+      <c r="D62" s="165"/>
       <c r="E62" s="17"/>
-      <c r="F62" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G62" s="144" t="s">
-        <v>204</v>
-      </c>
-      <c r="H62" s="140" t="s">
-        <v>205</v>
-      </c>
-      <c r="I62" s="145"/>
+      <c r="F62" s="124" t="s">
+        <v>202</v>
+      </c>
+      <c r="G62" s="120" t="s">
+        <v>203</v>
+      </c>
+      <c r="H62" s="125"/>
+      <c r="I62" s="5"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
+      <c r="M62" s="6"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
-      <c r="P62" s="6"/>
-    </row>
-    <row r="63" spans="1:16">
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
-      <c r="D63" s="101"/>
-      <c r="E63" s="110"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="151" t="s">
+      <c r="D63" s="166"/>
+      <c r="E63" s="92"/>
+      <c r="F63" s="130" t="s">
+        <v>204</v>
+      </c>
+      <c r="G63" s="128" t="s">
+        <v>205</v>
+      </c>
+      <c r="H63" s="134" t="s">
         <v>206</v>
       </c>
-      <c r="H63" s="148" t="s">
-        <v>207</v>
-      </c>
-      <c r="I63" s="155" t="s">
-        <v>208</v>
-      </c>
-      <c r="J63" s="155" t="s">
-        <v>208</v>
-      </c>
-      <c r="K63" s="155"/>
-      <c r="L63" s="97"/>
-      <c r="M63" s="97"/>
+      <c r="I63" s="134" t="s">
+        <v>206</v>
+      </c>
+      <c r="J63" s="134"/>
+      <c r="K63" s="81"/>
+      <c r="L63" s="81"/>
+      <c r="M63" s="6"/>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
-      <c r="P63" s="6"/>
-    </row>
-    <row r="64" spans="1:16">
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
-      <c r="D64" s="156" t="s">
+      <c r="D64" s="167" t="s">
+        <v>207</v>
+      </c>
+      <c r="E64" s="92"/>
+      <c r="F64" s="135" t="s">
+        <v>208</v>
+      </c>
+      <c r="G64" s="128" t="s">
         <v>209</v>
       </c>
-      <c r="E64" s="110"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="157" t="s">
+      <c r="H64" s="134" t="s">
         <v>210</v>
       </c>
-      <c r="H64" s="148" t="s">
+      <c r="I64" s="134" t="s">
         <v>211</v>
       </c>
-      <c r="I64" s="155" t="s">
+      <c r="J64" s="134" t="s">
         <v>212</v>
       </c>
-      <c r="J64" s="155" t="s">
-        <v>213</v>
-      </c>
-      <c r="K64" s="155" t="s">
-        <v>214</v>
-      </c>
-      <c r="L64" s="97"/>
-      <c r="M64" s="97"/>
+      <c r="K64" s="81"/>
+      <c r="L64" s="81"/>
+      <c r="M64" s="6"/>
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
-      <c r="P64" s="6"/>
-    </row>
-    <row r="65" spans="1:16">
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
-      <c r="D65" s="156"/>
-      <c r="E65" s="110"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="158" t="s">
-        <v>215</v>
-      </c>
-      <c r="H65" s="148" t="s">
-        <v>216</v>
-      </c>
-      <c r="I65" s="159" t="s">
-        <v>39</v>
-      </c>
-      <c r="J65" s="159" t="s">
-        <v>39</v>
-      </c>
-      <c r="K65" s="159" t="s">
-        <v>39</v>
-      </c>
-      <c r="L65" s="97"/>
-      <c r="M65" s="97"/>
+      <c r="D65" s="167"/>
+      <c r="E65" s="92"/>
+      <c r="F65" s="136" t="s">
+        <v>213</v>
+      </c>
+      <c r="G65" s="128" t="s">
+        <v>214</v>
+      </c>
+      <c r="H65" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="I65" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="J65" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="K65" s="81"/>
+      <c r="L65" s="81"/>
+      <c r="M65" s="6"/>
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
-      <c r="P65" s="6"/>
-    </row>
-    <row r="66" spans="1:16">
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
-      <c r="D66" s="156"/>
+      <c r="D66" s="167"/>
       <c r="E66" s="17"/>
-      <c r="F66" s="22"/>
-      <c r="G66" s="158" t="s">
+      <c r="F66" s="136" t="s">
+        <v>215</v>
+      </c>
+      <c r="G66" s="128" t="s">
+        <v>216</v>
+      </c>
+      <c r="H66" s="137" t="s">
         <v>217</v>
       </c>
-      <c r="H66" s="148" t="s">
-        <v>218</v>
-      </c>
-      <c r="I66" s="159" t="s">
-        <v>219</v>
-      </c>
-      <c r="J66" s="159" t="s">
-        <v>219</v>
-      </c>
-      <c r="K66" s="159" t="s">
-        <v>219</v>
-      </c>
-      <c r="L66" s="97"/>
-      <c r="M66" s="97"/>
+      <c r="I66" s="137" t="s">
+        <v>217</v>
+      </c>
+      <c r="J66" s="137" t="s">
+        <v>217</v>
+      </c>
+      <c r="K66" s="81"/>
+      <c r="L66" s="81"/>
+      <c r="M66" s="6"/>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
-      <c r="P66" s="6"/>
-    </row>
-    <row r="67" spans="1:16" ht="15" customHeight="1">
+    </row>
+    <row r="67" spans="1:15" ht="15" customHeight="1">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
-      <c r="D67" s="156"/>
+      <c r="D67" s="167"/>
       <c r="E67" s="17">
         <v>2</v>
       </c>
-      <c r="F67" s="22"/>
-      <c r="G67" s="160" t="s">
-        <v>220</v>
-      </c>
-      <c r="H67" s="161" t="s">
-        <v>221</v>
-      </c>
-      <c r="I67" s="162"/>
-      <c r="J67" s="162"/>
-      <c r="K67" s="162"/>
+      <c r="F67" s="138" t="s">
+        <v>218</v>
+      </c>
+      <c r="G67" s="139" t="s">
+        <v>219</v>
+      </c>
+      <c r="H67" s="140"/>
+      <c r="I67" s="140"/>
+      <c r="J67" s="140"/>
+      <c r="K67" s="5"/>
       <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
+      <c r="M67" s="6"/>
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
-      <c r="P67" s="6"/>
-    </row>
-    <row r="68" spans="1:16">
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
-      <c r="D68" s="156"/>
+      <c r="D68" s="167"/>
       <c r="E68" s="17">
         <v>1</v>
       </c>
-      <c r="F68" s="22"/>
-      <c r="G68" s="19" t="s">
+      <c r="F68" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="G68" s="139" t="s">
+        <v>221</v>
+      </c>
+      <c r="H68" s="60" t="s">
         <v>222</v>
       </c>
-      <c r="H68" s="161" t="s">
-        <v>223</v>
-      </c>
-      <c r="I68" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="J68" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="K68" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="L68" s="13"/>
-      <c r="M68" s="5"/>
+      <c r="I68" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="J68" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="K68" s="13"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="6"/>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
-      <c r="P68" s="6"/>
-    </row>
-    <row r="69" spans="1:16" s="6" customFormat="1">
-      <c r="D69" s="156"/>
+    </row>
+    <row r="69" spans="1:15" s="6" customFormat="1">
+      <c r="D69" s="167"/>
       <c r="E69" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="G69" s="139" t="s">
         <v>225</v>
       </c>
-      <c r="F69" s="22"/>
-      <c r="G69" s="19" t="s">
+      <c r="H69" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="H69" s="161" t="s">
+      <c r="I69" s="16">
+        <v>702880946</v>
+      </c>
+      <c r="J69" s="16">
+        <v>632085528</v>
+      </c>
+      <c r="K69" s="13"/>
+      <c r="L69" s="5"/>
+    </row>
+    <row r="70" spans="1:15" s="10" customFormat="1">
+      <c r="D70" s="167"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="I69" s="16" t="s">
+      <c r="G70" s="141" t="s">
         <v>228</v>
       </c>
-      <c r="J69" s="16">
-        <v>702880946</v>
-      </c>
-      <c r="K69" s="16">
-        <v>632085528</v>
-      </c>
-      <c r="L69" s="13"/>
-      <c r="M69" s="5"/>
-    </row>
-    <row r="70" spans="1:16" s="10" customFormat="1">
-      <c r="D70" s="156"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="20" t="s">
+      <c r="H70" s="142" t="s">
         <v>229</v>
       </c>
-      <c r="H70" s="163" t="s">
-        <v>230</v>
-      </c>
-      <c r="I70" s="164" t="s">
-        <v>231</v>
-      </c>
-      <c r="J70" s="164" t="s">
-        <v>231</v>
-      </c>
-      <c r="K70" s="164" t="s">
-        <v>231</v>
-      </c>
-      <c r="L70" s="14"/>
-      <c r="M70" s="11"/>
-    </row>
-    <row r="71" spans="1:16">
+      <c r="I70" s="142" t="s">
+        <v>229</v>
+      </c>
+      <c r="J70" s="142" t="s">
+        <v>229</v>
+      </c>
+      <c r="K70" s="14"/>
+      <c r="L70" s="11"/>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
-      <c r="D71" s="156"/>
+      <c r="D71" s="167"/>
       <c r="E71" s="17">
         <v>2</v>
       </c>
-      <c r="F71" s="22"/>
-      <c r="G71" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="H71" s="161" t="s">
-        <v>233</v>
-      </c>
-      <c r="I71" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="J71" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="K71" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="L71" s="13"/>
-      <c r="M71" s="5"/>
+      <c r="F71" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="G71" s="139" t="s">
+        <v>231</v>
+      </c>
+      <c r="H71" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="I71" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="J71" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="K71" s="13"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="6"/>
       <c r="N71" s="6"/>
       <c r="O71" s="6"/>
-      <c r="P71" s="6"/>
-    </row>
-    <row r="72" spans="1:16" s="6" customFormat="1">
-      <c r="D72" s="156"/>
+    </row>
+    <row r="72" spans="1:15" s="6" customFormat="1">
+      <c r="D72" s="167"/>
       <c r="E72" s="17">
         <v>2</v>
       </c>
-      <c r="F72" s="22"/>
-      <c r="G72" s="19" t="s">
+      <c r="F72" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="G72" s="139" t="s">
+        <v>233</v>
+      </c>
+      <c r="H72" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="I72" s="16">
+        <v>702880946</v>
+      </c>
+      <c r="J72" s="16">
+        <v>561964589</v>
+      </c>
+      <c r="K72" s="13"/>
+      <c r="L72" s="5"/>
+    </row>
+    <row r="73" spans="1:15" s="10" customFormat="1">
+      <c r="D73" s="167"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="H72" s="161" t="s">
+      <c r="G73" s="141" t="s">
         <v>235</v>
       </c>
-      <c r="I72" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="J72" s="16">
-        <v>702880946</v>
-      </c>
-      <c r="K72" s="16">
-        <v>561964589</v>
-      </c>
-      <c r="L72" s="13"/>
-      <c r="M72" s="5"/>
-    </row>
-    <row r="73" spans="1:16" s="10" customFormat="1">
-      <c r="D73" s="156"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="20" t="s">
+      <c r="H73" s="142" t="s">
+        <v>229</v>
+      </c>
+      <c r="I73" s="142" t="s">
+        <v>229</v>
+      </c>
+      <c r="J73" s="142" t="s">
+        <v>229</v>
+      </c>
+      <c r="K73" s="14"/>
+      <c r="L73" s="11"/>
+    </row>
+    <row r="74" spans="1:15" s="6" customFormat="1">
+      <c r="D74" s="167"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="H73" s="163" t="s">
+      <c r="G74" s="139" t="s">
         <v>237</v>
       </c>
-      <c r="I73" s="164" t="s">
-        <v>231</v>
-      </c>
-      <c r="J73" s="164" t="s">
-        <v>231</v>
-      </c>
-      <c r="K73" s="164" t="s">
-        <v>231</v>
-      </c>
-      <c r="L73" s="14"/>
-      <c r="M73" s="11"/>
-    </row>
-    <row r="74" spans="1:16" s="6" customFormat="1">
-      <c r="D74" s="156"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="22"/>
-      <c r="G74" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="H74" s="161" t="s">
-        <v>239</v>
-      </c>
-      <c r="I74" s="15" t="s">
-        <v>147</v>
+      <c r="H74" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I74" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="J74" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="K74" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="L74" s="13"/>
-      <c r="M74" s="5"/>
-    </row>
-    <row r="75" spans="1:16">
+        <v>146</v>
+      </c>
+      <c r="K74" s="13"/>
+      <c r="L74" s="5"/>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
-      <c r="D75" s="156"/>
+      <c r="D75" s="167"/>
       <c r="E75" s="17">
         <v>3</v>
       </c>
-      <c r="F75" s="22"/>
-      <c r="G75" s="19" t="s">
+      <c r="F75" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="G75" s="139" t="s">
+        <v>239</v>
+      </c>
+      <c r="H75" s="143" t="s">
         <v>240</v>
       </c>
-      <c r="H75" s="161" t="s">
+      <c r="I75" s="61" t="s">
         <v>241</v>
       </c>
-      <c r="I75" s="165" t="s">
-        <v>242</v>
-      </c>
-      <c r="J75" s="75" t="s">
-        <v>243</v>
-      </c>
-      <c r="K75" s="75" t="s">
-        <v>243</v>
-      </c>
-      <c r="L75" s="13"/>
-      <c r="M75" s="5"/>
+      <c r="J75" s="61" t="s">
+        <v>241</v>
+      </c>
+      <c r="K75" s="13"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="6"/>
       <c r="N75" s="6"/>
       <c r="O75" s="6"/>
-      <c r="P75" s="6"/>
-    </row>
-    <row r="76" spans="1:16">
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
-      <c r="D76" s="156"/>
+      <c r="D76" s="167"/>
       <c r="E76" s="17"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="H76" s="161" t="s">
-        <v>245</v>
-      </c>
-      <c r="I76" s="165"/>
-      <c r="J76" s="75"/>
-      <c r="K76" s="75"/>
-      <c r="L76" s="144"/>
-      <c r="M76" s="5"/>
+      <c r="F76" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G76" s="139" t="s">
+        <v>243</v>
+      </c>
+      <c r="H76" s="143"/>
+      <c r="I76" s="61"/>
+      <c r="J76" s="61"/>
+      <c r="K76" s="124"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="6"/>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
-      <c r="P76" s="6"/>
-    </row>
-    <row r="77" spans="1:16">
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
-      <c r="D77" s="156"/>
+      <c r="D77" s="167"/>
       <c r="E77" s="17"/>
-      <c r="F77" s="22"/>
-      <c r="G77" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="H77" s="161" t="s">
-        <v>247</v>
-      </c>
-      <c r="I77" s="74"/>
-      <c r="J77" s="75"/>
-      <c r="K77" s="75"/>
-      <c r="L77" s="19"/>
-      <c r="M77" s="13"/>
+      <c r="F77" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="G77" s="139" t="s">
+        <v>245</v>
+      </c>
+      <c r="H77" s="60"/>
+      <c r="I77" s="61"/>
+      <c r="J77" s="61"/>
+      <c r="K77" s="19"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="6"/>
       <c r="N77" s="6"/>
       <c r="O77" s="6"/>
-      <c r="P77" s="6"/>
-    </row>
-    <row r="78" spans="1:16" ht="30.75">
+    </row>
+    <row r="78" spans="1:15" ht="30.75">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
-      <c r="D78" s="156"/>
+      <c r="D78" s="167"/>
       <c r="E78" s="17">
         <v>2</v>
       </c>
-      <c r="F78" s="22"/>
-      <c r="G78" s="19" t="s">
+      <c r="F78" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="G78" s="139" t="s">
+        <v>247</v>
+      </c>
+      <c r="H78" s="144" t="s">
         <v>248</v>
       </c>
-      <c r="H78" s="161" t="s">
+      <c r="I78" s="144" t="s">
         <v>249</v>
       </c>
-      <c r="I78" s="166" t="s">
+      <c r="J78" s="144" t="s">
         <v>250</v>
       </c>
-      <c r="J78" s="166" t="s">
-        <v>251</v>
-      </c>
-      <c r="K78" s="166" t="s">
-        <v>252</v>
-      </c>
-      <c r="L78" s="75"/>
-      <c r="M78" s="13"/>
+      <c r="K78" s="61"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="6"/>
       <c r="N78" s="6"/>
       <c r="O78" s="6"/>
-      <c r="P78" s="6"/>
-    </row>
-    <row r="79" spans="1:16">
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
-      <c r="D79" s="156"/>
+      <c r="D79" s="167"/>
       <c r="E79" s="17"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="H79" s="161" t="s">
-        <v>254</v>
-      </c>
-      <c r="I79" s="27"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="75"/>
-      <c r="L79" s="75"/>
-      <c r="M79" s="13"/>
+      <c r="F79" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="G79" s="139" t="s">
+        <v>252</v>
+      </c>
+      <c r="H79" s="22"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="61"/>
+      <c r="K79" s="61"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="6"/>
       <c r="N79" s="6"/>
       <c r="O79" s="6"/>
-      <c r="P79" s="6"/>
-    </row>
-    <row r="80" spans="1:16">
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
-      <c r="D80" s="156"/>
+      <c r="D80" s="167"/>
       <c r="E80" s="17">
         <v>2</v>
       </c>
-      <c r="F80" s="22"/>
-      <c r="G80" s="19" t="s">
+      <c r="F80" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="G80" s="139" t="s">
+        <v>254</v>
+      </c>
+      <c r="H80" s="60" t="s">
         <v>255</v>
       </c>
-      <c r="H80" s="161" t="s">
+      <c r="I80" s="61" t="s">
         <v>256</v>
       </c>
-      <c r="I80" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="J80" s="75" t="s">
-        <v>258</v>
-      </c>
-      <c r="K80" s="19"/>
-      <c r="L80" s="75"/>
-      <c r="M80" s="13"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="61"/>
+      <c r="L80" s="13"/>
+      <c r="M80" s="6"/>
       <c r="N80" s="6"/>
       <c r="O80" s="6"/>
-      <c r="P80" s="6"/>
-    </row>
-    <row r="81" spans="1:16">
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
-      <c r="D81" s="156"/>
+      <c r="D81" s="167"/>
       <c r="E81" s="17"/>
-      <c r="F81" s="22"/>
-      <c r="G81" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="H81" s="161" t="s">
-        <v>260</v>
-      </c>
-      <c r="I81" s="74"/>
-      <c r="J81" s="75"/>
-      <c r="K81" s="19"/>
-      <c r="L81" s="75"/>
-      <c r="M81" s="13"/>
+      <c r="F81" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="G81" s="139" t="s">
+        <v>258</v>
+      </c>
+      <c r="H81" s="60"/>
+      <c r="I81" s="61"/>
+      <c r="J81" s="19"/>
+      <c r="K81" s="61"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="6"/>
       <c r="N81" s="6"/>
       <c r="O81" s="6"/>
-      <c r="P81" s="6"/>
-    </row>
-    <row r="82" spans="1:16">
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
-      <c r="D82" s="156"/>
+      <c r="D82" s="167"/>
       <c r="E82" s="17">
         <v>2</v>
       </c>
-      <c r="F82" s="22"/>
-      <c r="G82" s="19" t="s">
+      <c r="F82" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="G82" s="139" t="s">
+        <v>260</v>
+      </c>
+      <c r="H82" s="60"/>
+      <c r="I82" s="61" t="s">
         <v>261</v>
       </c>
-      <c r="H82" s="161" t="s">
-        <v>262</v>
-      </c>
-      <c r="I82" s="74"/>
-      <c r="J82" s="75" t="s">
-        <v>263</v>
-      </c>
-      <c r="K82" s="154"/>
-      <c r="L82" s="140"/>
-      <c r="M82" s="5"/>
+      <c r="J82" s="133"/>
+      <c r="K82" s="120"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="6"/>
       <c r="N82" s="6"/>
       <c r="O82" s="6"/>
-      <c r="P82" s="6"/>
-    </row>
-    <row r="83" spans="1:16">
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
-      <c r="D83" s="156"/>
+      <c r="D83" s="167"/>
       <c r="E83" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="F83" s="22"/>
-      <c r="G83" s="167" t="s">
+        <v>223</v>
+      </c>
+      <c r="F83" s="145" t="s">
+        <v>262</v>
+      </c>
+      <c r="G83" s="139" t="s">
+        <v>263</v>
+      </c>
+      <c r="H83" s="146" t="s">
         <v>264</v>
       </c>
-      <c r="H83" s="161" t="s">
+      <c r="I83" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="I83" s="168" t="s">
+      <c r="J83" s="93" t="s">
         <v>266</v>
       </c>
-      <c r="J83" s="168" t="s">
-        <v>267</v>
-      </c>
-      <c r="K83" s="111" t="s">
-        <v>268</v>
-      </c>
+      <c r="K83" s="5"/>
       <c r="L83" s="5"/>
-      <c r="M83" s="5"/>
+      <c r="M83" s="6"/>
       <c r="N83" s="6"/>
       <c r="O83" s="6"/>
-      <c r="P83" s="6"/>
-    </row>
-    <row r="84" spans="1:16">
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
-      <c r="D84" s="156"/>
+      <c r="D84" s="167"/>
       <c r="E84" s="17"/>
-      <c r="F84" s="22"/>
-      <c r="G84" s="19" t="s">
+      <c r="F84" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="G84" s="139" t="s">
+        <v>268</v>
+      </c>
+      <c r="H84" s="60" t="s">
         <v>269</v>
       </c>
-      <c r="H84" s="161" t="s">
+      <c r="I84" s="61" t="s">
         <v>270</v>
       </c>
-      <c r="I84" s="74" t="s">
+      <c r="J84" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="J84" s="75" t="s">
-        <v>272</v>
-      </c>
-      <c r="K84" s="13" t="s">
-        <v>273</v>
-      </c>
+      <c r="K84" s="5"/>
       <c r="L84" s="5"/>
-      <c r="M84" s="5"/>
+      <c r="M84" s="6"/>
       <c r="N84" s="6"/>
       <c r="O84" s="6"/>
-      <c r="P84" s="6"/>
-    </row>
-    <row r="85" spans="1:16">
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
-      <c r="D85" s="156"/>
+      <c r="D85" s="167"/>
       <c r="E85" s="17"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="169" t="s">
+      <c r="F85" s="147" t="s">
+        <v>272</v>
+      </c>
+      <c r="G85" s="148" t="s">
+        <v>273</v>
+      </c>
+      <c r="H85" s="149" t="s">
+        <v>123</v>
+      </c>
+      <c r="I85" s="150" t="s">
         <v>274</v>
       </c>
-      <c r="H85" s="170" t="s">
+      <c r="J85" s="125" t="s">
         <v>275</v>
       </c>
-      <c r="I85" s="171" t="s">
-        <v>124</v>
-      </c>
-      <c r="J85" s="172" t="s">
-        <v>276</v>
-      </c>
-      <c r="K85" s="145" t="s">
-        <v>277</v>
-      </c>
-      <c r="L85" s="145"/>
-      <c r="M85" s="145"/>
+      <c r="K85" s="125"/>
+      <c r="L85" s="125"/>
+      <c r="M85" s="6"/>
       <c r="N85" s="6"/>
       <c r="O85" s="6"/>
-      <c r="P85" s="6"/>
-    </row>
-    <row r="86" spans="1:16" s="9" customFormat="1">
-      <c r="A86" s="173"/>
-      <c r="B86" s="173"/>
-      <c r="C86" s="173"/>
-      <c r="D86" s="156"/>
-      <c r="E86" s="110"/>
-      <c r="F86" s="22"/>
-      <c r="G86" s="174" t="s">
+    </row>
+    <row r="86" spans="1:15" s="9" customFormat="1">
+      <c r="A86" s="151"/>
+      <c r="B86" s="151"/>
+      <c r="C86" s="151"/>
+      <c r="D86" s="167"/>
+      <c r="E86" s="92"/>
+      <c r="F86" s="152" t="s">
+        <v>276</v>
+      </c>
+      <c r="G86" s="153" t="s">
+        <v>277</v>
+      </c>
+      <c r="H86" s="130" t="s">
+        <v>95</v>
+      </c>
+      <c r="I86" s="130" t="s">
+        <v>96</v>
+      </c>
+      <c r="J86" s="130" t="s">
         <v>278</v>
       </c>
-      <c r="H86" s="175" t="s">
+      <c r="K86" s="154"/>
+      <c r="L86" s="154"/>
+      <c r="M86" s="151"/>
+      <c r="N86" s="151"/>
+      <c r="O86" s="151"/>
+    </row>
+    <row r="87" spans="1:15" s="9" customFormat="1">
+      <c r="A87" s="151"/>
+      <c r="B87" s="151"/>
+      <c r="C87" s="151"/>
+      <c r="D87" s="167"/>
+      <c r="E87" s="92"/>
+      <c r="F87" s="152" t="s">
         <v>279</v>
       </c>
-      <c r="I86" s="151" t="s">
-        <v>96</v>
-      </c>
-      <c r="J86" s="151" t="s">
-        <v>97</v>
-      </c>
-      <c r="K86" s="151" t="s">
+      <c r="G87" s="153" t="s">
         <v>280</v>
       </c>
-      <c r="L86" s="176"/>
-      <c r="M86" s="176"/>
-      <c r="N86" s="173"/>
-      <c r="O86" s="173"/>
-      <c r="P86" s="173"/>
-    </row>
-    <row r="87" spans="1:16" s="9" customFormat="1">
-      <c r="A87" s="173"/>
-      <c r="B87" s="173"/>
-      <c r="C87" s="173"/>
-      <c r="D87" s="156"/>
-      <c r="E87" s="110"/>
-      <c r="F87" s="22"/>
-      <c r="G87" s="174" t="s">
+      <c r="H87" s="155" t="s">
         <v>281</v>
       </c>
-      <c r="H87" s="175" t="s">
+      <c r="I87" s="155" t="s">
         <v>282</v>
       </c>
-      <c r="I87" s="177" t="s">
+      <c r="J87" s="155" t="s">
         <v>283</v>
       </c>
-      <c r="J87" s="177" t="s">
+      <c r="K87" s="154"/>
+      <c r="L87" s="154"/>
+      <c r="M87" s="151"/>
+      <c r="N87" s="151"/>
+      <c r="O87" s="151"/>
+    </row>
+    <row r="88" spans="1:15" s="7" customFormat="1">
+      <c r="A88" s="156" t="s">
         <v>284</v>
       </c>
-      <c r="K87" s="177" t="s">
-        <v>285</v>
-      </c>
-      <c r="L87" s="176"/>
-      <c r="M87" s="176"/>
-      <c r="N87" s="173"/>
-      <c r="O87" s="173"/>
-      <c r="P87" s="173"/>
-    </row>
-    <row r="88" spans="1:16" s="7" customFormat="1">
-      <c r="A88" s="178" t="s">
-        <v>286</v>
-      </c>
-      <c r="B88" s="178"/>
-      <c r="C88" s="178"/>
-      <c r="D88" s="178"/>
-      <c r="E88" s="179"/>
-      <c r="F88" s="180"/>
-      <c r="G88" s="178"/>
-      <c r="H88" s="178"/>
-      <c r="I88" s="181"/>
-      <c r="J88" s="178"/>
-      <c r="K88" s="178"/>
-      <c r="L88" s="178"/>
-      <c r="M88" s="178"/>
-      <c r="N88" s="178"/>
-      <c r="O88" s="178"/>
-      <c r="P88" s="178"/>
+      <c r="B88" s="156"/>
+      <c r="C88" s="156"/>
+      <c r="D88" s="156"/>
+      <c r="E88" s="157"/>
+      <c r="F88" s="156"/>
+      <c r="G88" s="156"/>
+      <c r="H88" s="158"/>
+      <c r="I88" s="156"/>
+      <c r="J88" s="156"/>
+      <c r="K88" s="156"/>
+      <c r="L88" s="156"/>
+      <c r="M88" s="156"/>
+      <c r="N88" s="156"/>
+      <c r="O88" s="156"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:P88" xr:uid="{FC96D3DE-56F6-4E60-B012-339ED5333B2B}">
+  <autoFilter ref="A9:O88" xr:uid="{FC96D3DE-56F6-4E60-B012-339ED5333B2B}">
     <filterColumn colId="0" showButton="0"/>
   </autoFilter>
   <mergeCells count="14">
-    <mergeCell ref="K2:P4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D18:D25"/>
     <mergeCell ref="D41:D63"/>
     <mergeCell ref="D64:D87"/>
     <mergeCell ref="D27:D33"/>
     <mergeCell ref="D34:D40"/>
-    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="D11:D15"/>
+    <mergeCell ref="J2:O4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="44" priority="93">
-      <formula>AND($AE27=1,$AD27=1)</formula>
+    <cfRule type="expression" dxfId="32" priority="93">
+      <formula>AND($AD27=1,$AC27=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="94">
-      <formula>$AE27=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="95">
-      <formula>OR($AE27="X",$AD27="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="96">
+    <cfRule type="expression" dxfId="31" priority="94">
       <formula>$AD27=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="97">
-      <formula>AND(NOT(ISBLANK($X27)),ISBLANK($AD27),ISBLANK($AE27))</formula>
+    <cfRule type="expression" dxfId="30" priority="95">
+      <formula>OR($AD27="X",$AC27="X")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="96">
+      <formula>$AC27=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="97">
+      <formula>AND(NOT(ISBLANK($W27)),ISBLANK($AC27),ISBLANK($AD27))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="39" priority="53">
-      <formula>AND($AE34=1,$AD34=1)</formula>
+    <cfRule type="expression" dxfId="27" priority="53">
+      <formula>AND($AD34=1,$AC34=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="54">
-      <formula>$AE34=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="55">
-      <formula>OR($AE34="X",$AD34="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="56">
+    <cfRule type="expression" dxfId="26" priority="54">
       <formula>$AD34=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="57">
-      <formula>AND(NOT(ISBLANK($X34)),ISBLANK($AD34),ISBLANK($AE34))</formula>
+    <cfRule type="expression" dxfId="25" priority="55">
+      <formula>OR($AD34="X",$AC34="X")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="56">
+      <formula>$AC34=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="57">
+      <formula>AND(NOT(ISBLANK($W34)),ISBLANK($AC34),ISBLANK($AD34))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="34" priority="88">
+    <cfRule type="expression" dxfId="22" priority="88">
       <formula>AND(#REF!=1,#REF!=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="89">
+    <cfRule type="expression" dxfId="21" priority="89">
       <formula>#REF!=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="90">
+    <cfRule type="expression" dxfId="20" priority="90">
       <formula>OR(#REF!="X",#REF!="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="91">
+    <cfRule type="expression" dxfId="19" priority="91">
       <formula>#REF!=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="92">
+    <cfRule type="expression" dxfId="18" priority="92">
       <formula>AND(NOT(ISBLANK(#REF!)),ISBLANK(#REF!),ISBLANK(#REF!))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="expression" dxfId="29" priority="104">
-      <formula>AND($S41="X",$B41&lt;&gt;"")</formula>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="expression" dxfId="17" priority="111">
+      <formula>AND($R41="X",$B41&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="105">
-      <formula>AND($AE41=1,$AD41=1)</formula>
+    <cfRule type="expression" dxfId="16" priority="112">
+      <formula>AND($AD41=1,$AC41=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="106">
-      <formula>$AE41=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="107">
-      <formula>OR($AE41="X",$AD41="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="108">
+    <cfRule type="expression" dxfId="15" priority="113">
       <formula>$AD41=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="109">
-      <formula>AND(NOT(ISBLANK($X41)),ISBLANK($AD41),ISBLANK($AE41))</formula>
+    <cfRule type="expression" dxfId="14" priority="114">
+      <formula>OR($AD41="X",$AC41="X")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="115">
+      <formula>$AC41=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="116">
+      <formula>AND(NOT(ISBLANK($W41)),ISBLANK($AC41),ISBLANK($AD41))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G64:G67 H67:H85">
-    <cfRule type="expression" dxfId="23" priority="77">
-      <formula>AND($AE64=1,$AD64=1)</formula>
+  <conditionalFormatting sqref="F64:F67 G67:G85">
+    <cfRule type="expression" dxfId="11" priority="117">
+      <formula>AND($AD64=1,$AC64=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="78">
-      <formula>$AE64=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="79">
-      <formula>OR($AE64="X",$AD64="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="80">
+    <cfRule type="expression" dxfId="10" priority="118">
       <formula>$AD64=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="81">
-      <formula>AND(NOT(ISBLANK($X64)),ISBLANK($AD64),ISBLANK($AE64))</formula>
+    <cfRule type="expression" dxfId="9" priority="119">
+      <formula>OR($AD64="X",$AC64="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="110">
-      <formula>AND($S64="X",$B64&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="8" priority="120">
+      <formula>$AC64=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="121">
+      <formula>AND(NOT(ISBLANK($W64)),ISBLANK($AC64),ISBLANK($AD64))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="122">
+      <formula>AND($R64="X",$B64&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G57:K57">
-    <cfRule type="expression" dxfId="17" priority="58">
-      <formula>AND($T57="X",OR($B57&lt;&gt;"",$D57&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="F57:J57 G58:G59 G63:G66">
+    <cfRule type="expression" dxfId="5" priority="129">
+      <formula>AND($S57="X",OR($B57&lt;&gt;"",$D57&lt;&gt;""))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="59">
-      <formula>AND($AF57=1,$AE57=1)</formula>
+    <cfRule type="expression" dxfId="4" priority="130">
+      <formula>AND($AE57=1,$AD57=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="60">
-      <formula>$AF57=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="61">
-      <formula>OR($AF57="X",$AE57="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="62">
+    <cfRule type="expression" dxfId="3" priority="131">
       <formula>$AE57=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="63">
-      <formula>AND(NOT(ISBLANK($Y57)),ISBLANK($AE57),ISBLANK($AF57))</formula>
+    <cfRule type="expression" dxfId="2" priority="132">
+      <formula>OR($AE57="X",$AD57="X")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H58:H59">
-    <cfRule type="expression" dxfId="11" priority="47">
-      <formula>AND($T58="X",OR($B58&lt;&gt;"",$D58&lt;&gt;""))</formula>
+    <cfRule type="expression" dxfId="1" priority="133">
+      <formula>$AD57=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="48">
-      <formula>AND($AF58=1,$AE58=1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="49">
-      <formula>$AF58=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="50">
-      <formula>OR($AF58="X",$AE58="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="51">
-      <formula>$AE58=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="52">
-      <formula>AND(NOT(ISBLANK($Y58)),ISBLANK($AE58),ISBLANK($AF58))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H63:H66">
-    <cfRule type="expression" dxfId="5" priority="41">
-      <formula>AND($T63="X",OR($B63&lt;&gt;"",$D63&lt;&gt;""))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="42">
-      <formula>AND($AF63=1,$AE63=1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="43">
-      <formula>$AF63=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="44">
-      <formula>OR($AF63="X",$AE63="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="45">
-      <formula>$AE63=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="46">
-      <formula>AND(NOT(ISBLANK($Y63)),ISBLANK($AE63),ISBLANK($AF63))</formula>
+    <cfRule type="expression" dxfId="0" priority="134">
+      <formula>AND(NOT(ISBLANK($X57)),ISBLANK($AD57),ISBLANK($AE57))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -5205,67 +4938,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5679,8 +5351,69 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33493A62-AC11-48A7-B6C8-0591C55C368B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AEC75D3-A67D-4574-BB93-839AC9299105}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5688,5 +5421,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AEC75D3-A67D-4574-BB93-839AC9299105}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33493A62-AC11-48A7-B6C8-0591C55C368B}"/>
 </file>
</xml_diff>

<commit_message>
feature/test-generator: fix excel file
</commit_message>
<xml_diff>
--- a/csv_parser/test-cases-15-15.xlsx
+++ b/csv_parser/test-cases-15-15.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ans-repos\SAMU-Hub-Modeles\csv_parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/13 - 15-15/04 - Pilotes 15-15/04 - JDD recette/JSON pour interface LRM/03 - Automodel tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507A43C-1400-417F-A71E-05F498B52338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE9CDEF5-7CDC-46F5-B434-661C7097DB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E95E427-60E8-4C01-A0F5-EF6B52DBDF48}"/>
+    <workbookView xWindow="3285" yWindow="1590" windowWidth="22740" windowHeight="12930" xr2:uid="{8E95E427-60E8-4C01-A0F5-EF6B52DBDF48}"/>
   </bookViews>
   <sheets>
     <sheet name="Partage de dossier simple" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Partage de dossier simple'!$A$9:$O$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Partage de dossier simple'!$A$9:$O$88</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,9 +46,9 @@
   <commentList>
     <comment ref="F65" authorId="0" shapeId="0" xr:uid="{FB75C0C9-7A43-4C0C-BF65-EEEEE383A568}">
       <text>
-        <t>[Commentaire à thread]
-Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
-Commentaire :
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Pour savoir quelle alerte utiliser dans une affaire :
 =&gt; Regarder cette date de réception</t>
       </text>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="285">
   <si>
     <t>Périmètre</t>
   </si>
@@ -792,6 +792,60 @@
     <t>$.createCaseHealth.initialAlert.caller.communication</t>
   </si>
   <si>
+    <t>datetime observations ARM 01</t>
+  </si>
+  <si>
+    <t>$.createCaseHealth.initialAlert.notes[0].creation</t>
+  </si>
+  <si>
+    <t>Infos / observations ARM 01</t>
+  </si>
+  <si>
+    <t>$.createCaseHealth.initialAlert.notes[0].freetext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupure grave causée par une scie circulaire au niveau de la main; saigne beaucoup. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entorse de la cheville, avec possible fracture. </t>
+  </si>
+  <si>
+    <t>Confusion, étourdissements, s’exprime difficilement</t>
+  </si>
+  <si>
+    <t>datetime observations ARM 02</t>
+  </si>
+  <si>
+    <t>$.createCaseHealth.initialAlert.notes[1].creation</t>
+  </si>
+  <si>
+    <t>Infos / observations ARM 02</t>
+  </si>
+  <si>
+    <t>$.createCaseHealth.initialAlert.notes[1].freetext</t>
+  </si>
+  <si>
+    <t>La victime est inconsciente (perte de connaissance).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheville gonflée et douloureuse. </t>
+  </si>
+  <si>
+    <t>datetime observations ARM 03</t>
+  </si>
+  <si>
+    <t>$.createCaseHealth.initialAlert.notes[2].creation</t>
+  </si>
+  <si>
+    <t>Infos / observations ARM 03</t>
+  </si>
+  <si>
+    <t>$.createCaseHealth.initialAlert.notes[2].freetext</t>
+  </si>
+  <si>
+    <t>Marche impossible.</t>
+  </si>
+  <si>
     <t>Prénom et nom du requérant</t>
   </si>
   <si>
@@ -837,6 +891,9 @@
     <t>Agent/service d'urgence</t>
   </si>
   <si>
+    <t>$.createCaseHealth.initialAlert.callTaker.organization</t>
+  </si>
+  <si>
     <t>fr.health.samu090</t>
   </si>
   <si>
@@ -856,16 +913,13 @@
   </si>
   <si>
     <t>End</t>
-  </si>
-  <si>
-    <t>$.createCaseHealth.initialAlert.callTaker.organization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,7 +1072,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1178,6 +1232,19 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1549,7 +1616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1577,14 +1644,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1609,11 +1676,11 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1622,43 +1689,43 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1669,13 +1736,13 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1684,7 +1751,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1692,7 +1759,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1715,20 +1782,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1736,40 +1803,40 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1784,35 +1851,35 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1828,40 +1895,73 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1870,36 +1970,6 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2163,9 +2233,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2203,7 +2273,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2309,7 +2379,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2451,7 +2521,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2468,16 +2538,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC96D3DE-56F6-4E60-B012-339ED5333B2B}">
-  <dimension ref="A1:O82"/>
+  <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="10" topLeftCell="G61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="10" topLeftCell="G73" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="G78" sqref="G78"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -2492,7 +2562,7 @@
     <col min="12" max="12" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="18.75">
       <c r="A1" s="159" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2583,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="18.75">
       <c r="A2" s="159" t="s">
         <v>2</v>
       </c>
@@ -2529,16 +2599,16 @@
       <c r="I2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="158" t="s">
+      <c r="J2" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="158"/>
-      <c r="L2" s="158"/>
-      <c r="M2" s="158"/>
-      <c r="N2" s="158"/>
-      <c r="O2" s="158"/>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K2" s="170"/>
+      <c r="L2" s="170"/>
+      <c r="M2" s="170"/>
+      <c r="N2" s="170"/>
+      <c r="O2" s="170"/>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="18.75">
       <c r="A3" s="159" t="s">
         <v>6</v>
       </c>
@@ -2552,14 +2622,14 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="158"/>
-      <c r="K3" s="158"/>
-      <c r="L3" s="158"/>
-      <c r="M3" s="158"/>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J3" s="170"/>
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
+      <c r="M3" s="170"/>
+      <c r="N3" s="170"/>
+      <c r="O3" s="170"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="18.75">
       <c r="A4" s="159" t="s">
         <v>7</v>
       </c>
@@ -2573,22 +2643,22 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
       <c r="I4" s="23"/>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158"/>
-      <c r="L4" s="158"/>
-      <c r="M4" s="158"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="170" t="s">
+      <c r="J4" s="170"/>
+      <c r="K4" s="170"/>
+      <c r="L4" s="170"/>
+      <c r="M4" s="170"/>
+      <c r="N4" s="170"/>
+      <c r="O4" s="170"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A5" s="167" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
+      <c r="F5" s="167"/>
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
       <c r="I5" s="23"/>
@@ -2599,13 +2669,13 @@
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="160" t="s">
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A6" s="171" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="161"/>
-      <c r="C6" s="161"/>
-      <c r="D6" s="162"/>
+      <c r="B6" s="172"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="173"/>
       <c r="E6" s="21"/>
       <c r="F6" s="6" t="s">
         <v>11</v>
@@ -2620,13 +2690,13 @@
       <c r="N6" s="26"/>
       <c r="O6" s="26"/>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="171" t="s">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="18.75">
+      <c r="A7" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="171"/>
-      <c r="C7" s="171"/>
-      <c r="D7" s="171"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="168"/>
+      <c r="D7" s="168"/>
       <c r="E7" s="27"/>
       <c r="F7" s="6" t="s">
         <v>13</v>
@@ -2641,7 +2711,7 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="18.75">
       <c r="A8" s="28"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -2660,7 +2730,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
     </row>
-    <row r="9" spans="1:15" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="2" customFormat="1" ht="18.75">
       <c r="A9" s="29" t="s">
         <v>15</v>
       </c>
@@ -2701,7 +2771,7 @@
       <c r="N9" s="36"/>
       <c r="O9" s="36"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="36" t="s">
         <v>26</v>
       </c>
@@ -2726,11 +2796,11 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="16.5" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="172" t="s">
+      <c r="D11" s="169" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="42"/>
@@ -2755,11 +2825,11 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="172"/>
+      <c r="D12" s="169"/>
       <c r="E12" s="42"/>
       <c r="F12" s="47" t="s">
         <v>36</v>
@@ -2782,11 +2852,11 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="172"/>
+      <c r="D13" s="169"/>
       <c r="E13" s="42"/>
       <c r="F13" s="51" t="s">
         <v>39</v>
@@ -2809,11 +2879,11 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="4" customFormat="1">
       <c r="A14" s="52"/>
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
-      <c r="D14" s="172"/>
+      <c r="D14" s="169"/>
       <c r="E14" s="17">
         <v>3</v>
       </c>
@@ -2838,11 +2908,11 @@
       <c r="N14" s="52"/>
       <c r="O14" s="52"/>
     </row>
-    <row r="15" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="4" customFormat="1">
       <c r="A15" s="52"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
-      <c r="D15" s="172"/>
+      <c r="D15" s="169"/>
       <c r="E15" s="17">
         <v>3</v>
       </c>
@@ -2867,7 +2937,7 @@
       <c r="N15" s="52"/>
       <c r="O15" s="52"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2890,7 +2960,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2913,11 +2983,11 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="163" t="s">
+      <c r="D18" s="160" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="42">
@@ -2944,11 +3014,11 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="28.5" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="164"/>
+      <c r="D19" s="161"/>
       <c r="E19" s="42">
         <v>3</v>
       </c>
@@ -2973,11 +3043,11 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="164"/>
+      <c r="D20" s="161"/>
       <c r="E20" s="17">
         <v>2</v>
       </c>
@@ -3002,11 +3072,11 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="8" customFormat="1" ht="30.75">
       <c r="A21" s="75"/>
       <c r="B21" s="75"/>
       <c r="C21" s="75"/>
-      <c r="D21" s="164"/>
+      <c r="D21" s="161"/>
       <c r="E21" s="76">
         <v>3</v>
       </c>
@@ -3031,11 +3101,11 @@
       <c r="N21" s="75"/>
       <c r="O21" s="75"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="164"/>
+      <c r="D22" s="161"/>
       <c r="E22" s="17">
         <v>1</v>
       </c>
@@ -3060,11 +3130,11 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
     </row>
-    <row r="23" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="30.75" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="164"/>
+      <c r="D23" s="161"/>
       <c r="E23" s="76">
         <v>3</v>
       </c>
@@ -3089,11 +3159,11 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="164"/>
+      <c r="D24" s="161"/>
       <c r="E24" s="17">
         <v>1</v>
       </c>
@@ -3118,11 +3188,11 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="165"/>
+      <c r="D25" s="162"/>
       <c r="E25" s="85">
         <v>3</v>
       </c>
@@ -3147,7 +3217,7 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -3178,11 +3248,11 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="167" t="s">
+      <c r="D27" s="164" t="s">
         <v>98</v>
       </c>
       <c r="E27" s="92"/>
@@ -3207,11 +3277,11 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="168"/>
+      <c r="D28" s="165"/>
       <c r="E28" s="17">
         <v>1</v>
       </c>
@@ -3236,8 +3306,8 @@
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="168"/>
+    <row r="29" spans="1:15" s="6" customFormat="1">
+      <c r="D29" s="165"/>
       <c r="E29" s="17">
         <v>2</v>
       </c>
@@ -3257,11 +3327,11 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="168"/>
+      <c r="D30" s="165"/>
       <c r="E30" s="17">
         <v>1</v>
       </c>
@@ -3284,11 +3354,11 @@
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="168"/>
+      <c r="D31" s="165"/>
       <c r="E31" s="17"/>
       <c r="F31" s="13" t="s">
         <v>117</v>
@@ -3309,11 +3379,11 @@
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="168"/>
+      <c r="D32" s="165"/>
       <c r="E32" s="17"/>
       <c r="F32" s="13" t="s">
         <v>121</v>
@@ -3334,11 +3404,11 @@
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
     </row>
-    <row r="33" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="4" customFormat="1">
       <c r="A33" s="52"/>
       <c r="B33" s="52"/>
       <c r="C33" s="52"/>
-      <c r="D33" s="168"/>
+      <c r="D33" s="165"/>
       <c r="E33" s="17">
         <v>2</v>
       </c>
@@ -3363,11 +3433,11 @@
       <c r="N33" s="52"/>
       <c r="O33" s="52"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="167" t="s">
+      <c r="D34" s="164" t="s">
         <v>130</v>
       </c>
       <c r="E34" s="92"/>
@@ -3386,11 +3456,11 @@
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="168"/>
+      <c r="D35" s="165"/>
       <c r="E35" s="17"/>
       <c r="F35" s="13" t="s">
         <v>104</v>
@@ -3407,11 +3477,11 @@
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="168"/>
+      <c r="D36" s="165"/>
       <c r="E36" s="17"/>
       <c r="F36" s="13" t="s">
         <v>109</v>
@@ -3428,11 +3498,11 @@
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="168"/>
+      <c r="D37" s="165"/>
       <c r="E37" s="17"/>
       <c r="F37" s="13" t="s">
         <v>113</v>
@@ -3449,11 +3519,11 @@
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="168"/>
+      <c r="D38" s="165"/>
       <c r="E38" s="17"/>
       <c r="F38" s="13" t="s">
         <v>117</v>
@@ -3470,11 +3540,11 @@
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="168"/>
+      <c r="D39" s="165"/>
       <c r="E39" s="17"/>
       <c r="F39" s="13" t="s">
         <v>121</v>
@@ -3491,11 +3561,11 @@
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
-      <c r="D40" s="169"/>
+      <c r="D40" s="166"/>
       <c r="E40" s="17"/>
       <c r="F40" s="105" t="s">
         <v>125</v>
@@ -3512,11 +3582,11 @@
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="163" t="s">
+      <c r="D41" s="160" t="s">
         <v>138</v>
       </c>
       <c r="E41" s="42"/>
@@ -3541,11 +3611,11 @@
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
-      <c r="D42" s="164"/>
+      <c r="D42" s="161"/>
       <c r="E42" s="17">
         <v>2</v>
       </c>
@@ -3570,11 +3640,11 @@
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
     </row>
-    <row r="43" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="4" customFormat="1">
       <c r="A43" s="52"/>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>
-      <c r="D43" s="164"/>
+      <c r="D43" s="161"/>
       <c r="E43" s="17"/>
       <c r="F43" s="114" t="s">
         <v>147</v>
@@ -3593,11 +3663,11 @@
       <c r="N43" s="52"/>
       <c r="O43" s="52"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="164"/>
+      <c r="D44" s="161"/>
       <c r="E44" s="92">
         <v>1</v>
       </c>
@@ -3622,11 +3692,11 @@
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
-      <c r="D45" s="164"/>
+      <c r="D45" s="161"/>
       <c r="E45" s="17">
         <v>1</v>
       </c>
@@ -3651,11 +3721,11 @@
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="164"/>
+      <c r="D46" s="161"/>
       <c r="E46" s="17">
         <v>3</v>
       </c>
@@ -3680,11 +3750,11 @@
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
-      <c r="D47" s="164"/>
+      <c r="D47" s="161"/>
       <c r="E47" s="17">
         <v>2</v>
       </c>
@@ -3705,11 +3775,11 @@
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
-      <c r="D48" s="164"/>
+      <c r="D48" s="161"/>
       <c r="E48" s="17">
         <v>2</v>
       </c>
@@ -3728,11 +3798,11 @@
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="164"/>
+      <c r="D49" s="161"/>
       <c r="E49" s="17">
         <v>2</v>
       </c>
@@ -3753,11 +3823,11 @@
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
-      <c r="D50" s="164"/>
+      <c r="D50" s="161"/>
       <c r="E50" s="17">
         <v>2</v>
       </c>
@@ -3778,11 +3848,11 @@
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
-      <c r="D51" s="164"/>
+      <c r="D51" s="161"/>
       <c r="E51" s="17">
         <v>2</v>
       </c>
@@ -3803,11 +3873,11 @@
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
-      <c r="D52" s="164"/>
+      <c r="D52" s="161"/>
       <c r="E52" s="17">
         <v>2</v>
       </c>
@@ -3828,11 +3898,11 @@
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
-      <c r="D53" s="164"/>
+      <c r="D53" s="161"/>
       <c r="E53" s="17">
         <v>2</v>
       </c>
@@ -3851,11 +3921,11 @@
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
-      <c r="D54" s="164"/>
+      <c r="D54" s="161"/>
       <c r="E54" s="17">
         <v>2</v>
       </c>
@@ -3874,11 +3944,11 @@
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
-      <c r="D55" s="164"/>
+      <c r="D55" s="161"/>
       <c r="E55" s="17">
         <v>2</v>
       </c>
@@ -3899,11 +3969,11 @@
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
     </row>
-    <row r="56" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="4" customFormat="1">
       <c r="A56" s="52"/>
       <c r="B56" s="52"/>
       <c r="C56" s="52"/>
-      <c r="D56" s="164"/>
+      <c r="D56" s="161"/>
       <c r="E56" s="17">
         <v>2</v>
       </c>
@@ -3928,11 +3998,11 @@
       <c r="N56" s="52"/>
       <c r="O56" s="52"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
-      <c r="D57" s="164"/>
+      <c r="D57" s="161"/>
       <c r="E57" s="92"/>
       <c r="F57" s="127" t="s">
         <v>187</v>
@@ -3953,11 +4023,11 @@
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="164"/>
+      <c r="D58" s="161"/>
       <c r="E58" s="92">
         <v>3</v>
       </c>
@@ -3980,11 +4050,11 @@
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
-      <c r="D59" s="164"/>
+      <c r="D59" s="161"/>
       <c r="E59" s="92">
         <v>3</v>
       </c>
@@ -4007,11 +4077,11 @@
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
-      <c r="D60" s="164"/>
+      <c r="D60" s="161"/>
       <c r="E60" s="17"/>
       <c r="F60" s="133" t="s">
         <v>198</v>
@@ -4028,11 +4098,11 @@
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
-      <c r="D61" s="164"/>
+      <c r="D61" s="161"/>
       <c r="E61" s="17"/>
       <c r="F61" s="13" t="s">
         <v>200</v>
@@ -4049,11 +4119,11 @@
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
-      <c r="D62" s="164"/>
+      <c r="D62" s="161"/>
       <c r="E62" s="17"/>
       <c r="F62" s="124" t="s">
         <v>202</v>
@@ -4070,11 +4140,11 @@
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
-      <c r="D63" s="165"/>
+      <c r="D63" s="162"/>
       <c r="E63" s="92"/>
       <c r="F63" s="130" t="s">
         <v>204</v>
@@ -4095,11 +4165,11 @@
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
-      <c r="D64" s="166" t="s">
+      <c r="D64" s="163" t="s">
         <v>207</v>
       </c>
       <c r="E64" s="92"/>
@@ -4124,11 +4194,11 @@
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
-      <c r="D65" s="166"/>
+      <c r="D65" s="163"/>
       <c r="E65" s="92"/>
       <c r="F65" s="136" t="s">
         <v>213</v>
@@ -4151,11 +4221,11 @@
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
-      <c r="D66" s="166"/>
+      <c r="D66" s="163"/>
       <c r="E66" s="17"/>
       <c r="F66" s="136" t="s">
         <v>215</v>
@@ -4178,11 +4248,11 @@
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="15" customHeight="1">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
-      <c r="D67" s="166"/>
+      <c r="D67" s="163"/>
       <c r="E67" s="17">
         <v>2</v>
       </c>
@@ -4201,11 +4271,11 @@
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
-      <c r="D68" s="166"/>
+      <c r="D68" s="163"/>
       <c r="E68" s="17">
         <v>1</v>
       </c>
@@ -4230,8 +4300,8 @@
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
     </row>
-    <row r="69" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D69" s="166"/>
+    <row r="69" spans="1:15" s="6" customFormat="1">
+      <c r="D69" s="163"/>
       <c r="E69" s="17" t="s">
         <v>223</v>
       </c>
@@ -4253,8 +4323,8 @@
       <c r="K69" s="13"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D70" s="166"/>
+    <row r="70" spans="1:15" s="10" customFormat="1">
+      <c r="D70" s="163"/>
       <c r="E70" s="18"/>
       <c r="F70" s="20" t="s">
         <v>227</v>
@@ -4274,11 +4344,11 @@
       <c r="K70" s="14"/>
       <c r="L70" s="11"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
-      <c r="D71" s="166"/>
+      <c r="D71" s="163"/>
       <c r="E71" s="17">
         <v>2</v>
       </c>
@@ -4303,8 +4373,8 @@
       <c r="N71" s="6"/>
       <c r="O71" s="6"/>
     </row>
-    <row r="72" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="166"/>
+    <row r="72" spans="1:15" s="6" customFormat="1">
+      <c r="D72" s="163"/>
       <c r="E72" s="17">
         <v>2</v>
       </c>
@@ -4326,8 +4396,8 @@
       <c r="K72" s="13"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D73" s="166"/>
+    <row r="73" spans="1:15" s="10" customFormat="1">
+      <c r="D73" s="163"/>
       <c r="E73" s="18"/>
       <c r="F73" s="20" t="s">
         <v>234</v>
@@ -4347,8 +4417,8 @@
       <c r="K73" s="14"/>
       <c r="L73" s="11"/>
     </row>
-    <row r="74" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D74" s="166"/>
+    <row r="74" spans="1:15" s="6" customFormat="1">
+      <c r="D74" s="163"/>
       <c r="E74" s="17"/>
       <c r="F74" s="19" t="s">
         <v>236</v>
@@ -4368,11 +4438,11 @@
       <c r="K74" s="13"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
-      <c r="D75" s="166"/>
+      <c r="D75" s="163"/>
       <c r="E75" s="17">
         <v>3</v>
       </c>
@@ -4397,11 +4467,11 @@
       <c r="N75" s="6"/>
       <c r="O75" s="6"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
-      <c r="D76" s="166"/>
+      <c r="D76" s="163"/>
       <c r="E76" s="17"/>
       <c r="F76" s="19" t="s">
         <v>242</v>
@@ -4418,181 +4488,325 @@
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
-      <c r="D77" s="166"/>
-      <c r="E77" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="F77" s="144" t="s">
+      <c r="D77" s="163"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="19" t="s">
         <v>244</v>
       </c>
       <c r="G77" s="139" t="s">
         <v>245</v>
       </c>
-      <c r="H77" s="145" t="s">
-        <v>246</v>
-      </c>
-      <c r="I77" s="145" t="s">
-        <v>247</v>
-      </c>
-      <c r="J77" s="93" t="s">
-        <v>248</v>
-      </c>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
+      <c r="H77" s="60"/>
+      <c r="I77" s="61"/>
+      <c r="J77" s="61"/>
+      <c r="K77" s="19"/>
+      <c r="L77" s="13"/>
       <c r="M77" s="6"/>
       <c r="N77" s="6"/>
       <c r="O77" s="6"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="30.75">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
-      <c r="D78" s="166"/>
-      <c r="E78" s="17"/>
+      <c r="D78" s="163"/>
+      <c r="E78" s="17">
+        <v>2</v>
+      </c>
       <c r="F78" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="G78" s="139" t="s">
+        <v>247</v>
+      </c>
+      <c r="H78" s="144" t="s">
+        <v>248</v>
+      </c>
+      <c r="I78" s="144" t="s">
         <v>249</v>
       </c>
-      <c r="G78" s="139" t="s">
+      <c r="J78" s="144" t="s">
         <v>250</v>
       </c>
-      <c r="H78" s="60" t="s">
-        <v>251</v>
-      </c>
-      <c r="I78" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="J78" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
+      <c r="K78" s="61"/>
+      <c r="L78" s="13"/>
       <c r="M78" s="6"/>
       <c r="N78" s="6"/>
       <c r="O78" s="6"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
-      <c r="D79" s="166"/>
+      <c r="D79" s="163"/>
       <c r="E79" s="17"/>
-      <c r="F79" s="146" t="s">
-        <v>254</v>
-      </c>
-      <c r="G79" s="147" t="s">
-        <v>255</v>
-      </c>
-      <c r="H79" s="148" t="s">
-        <v>123</v>
-      </c>
-      <c r="I79" s="149" t="s">
-        <v>256</v>
-      </c>
-      <c r="J79" s="125" t="s">
-        <v>257</v>
-      </c>
-      <c r="K79" s="125"/>
-      <c r="L79" s="125"/>
+      <c r="F79" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="G79" s="139" t="s">
+        <v>252</v>
+      </c>
+      <c r="H79" s="22"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="61"/>
+      <c r="K79" s="61"/>
+      <c r="L79" s="13"/>
       <c r="M79" s="6"/>
       <c r="N79" s="6"/>
       <c r="O79" s="6"/>
     </row>
-    <row r="80" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="150"/>
-      <c r="B80" s="150"/>
-      <c r="C80" s="150"/>
-      <c r="D80" s="166"/>
-      <c r="E80" s="92"/>
-      <c r="F80" s="151" t="s">
+    <row r="80" spans="1:15">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="163"/>
+      <c r="E80" s="17">
+        <v>2</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="G80" s="139" t="s">
+        <v>254</v>
+      </c>
+      <c r="H80" s="60" t="s">
+        <v>255</v>
+      </c>
+      <c r="I80" s="61" t="s">
+        <v>256</v>
+      </c>
+      <c r="J80" s="19"/>
+      <c r="K80" s="61"/>
+      <c r="L80" s="13"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+    </row>
+    <row r="81" spans="1:15">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="163"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="G81" s="139" t="s">
         <v>258</v>
       </c>
-      <c r="G80" s="152" t="s">
+      <c r="H81" s="60"/>
+      <c r="I81" s="61"/>
+      <c r="J81" s="19"/>
+      <c r="K81" s="61"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+    </row>
+    <row r="82" spans="1:15" ht="14.25" customHeight="1">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="163"/>
+      <c r="E82" s="17">
+        <v>2</v>
+      </c>
+      <c r="F82" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="G82" s="139" t="s">
+        <v>260</v>
+      </c>
+      <c r="H82" s="60"/>
+      <c r="I82" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="J82" s="133"/>
+      <c r="K82" s="120"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+    </row>
+    <row r="83" spans="1:15">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="163"/>
+      <c r="E83" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F83" s="145" t="s">
+        <v>262</v>
+      </c>
+      <c r="G83" s="139" t="s">
+        <v>263</v>
+      </c>
+      <c r="H83" s="146" t="s">
+        <v>264</v>
+      </c>
+      <c r="I83" s="146" t="s">
+        <v>265</v>
+      </c>
+      <c r="J83" s="93" t="s">
         <v>266</v>
       </c>
-      <c r="H80" s="130" t="s">
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+    </row>
+    <row r="84" spans="1:15">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="163"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="G84" s="139" t="s">
+        <v>268</v>
+      </c>
+      <c r="H84" s="60" t="s">
+        <v>269</v>
+      </c>
+      <c r="I84" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="J84" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+    </row>
+    <row r="85" spans="1:15">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="163"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="147" t="s">
+        <v>272</v>
+      </c>
+      <c r="G85" s="148" t="s">
+        <v>273</v>
+      </c>
+      <c r="H85" s="149" t="s">
+        <v>123</v>
+      </c>
+      <c r="I85" s="150" t="s">
+        <v>274</v>
+      </c>
+      <c r="J85" s="125" t="s">
+        <v>275</v>
+      </c>
+      <c r="K85" s="125"/>
+      <c r="L85" s="125"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+    </row>
+    <row r="86" spans="1:15" s="9" customFormat="1">
+      <c r="A86" s="151"/>
+      <c r="B86" s="151"/>
+      <c r="C86" s="151"/>
+      <c r="D86" s="163"/>
+      <c r="E86" s="92"/>
+      <c r="F86" s="152" t="s">
+        <v>276</v>
+      </c>
+      <c r="G86" s="153" t="s">
+        <v>277</v>
+      </c>
+      <c r="H86" s="130" t="s">
         <v>95</v>
       </c>
-      <c r="I80" s="130" t="s">
+      <c r="I86" s="130" t="s">
         <v>96</v>
       </c>
-      <c r="J80" s="130" t="s">
-        <v>259</v>
-      </c>
-      <c r="K80" s="153"/>
-      <c r="L80" s="153"/>
-      <c r="M80" s="150"/>
-      <c r="N80" s="150"/>
-      <c r="O80" s="150"/>
-    </row>
-    <row r="81" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="150"/>
-      <c r="B81" s="150"/>
-      <c r="C81" s="150"/>
-      <c r="D81" s="166"/>
-      <c r="E81" s="92"/>
-      <c r="F81" s="151" t="s">
-        <v>260</v>
-      </c>
-      <c r="G81" s="152" t="s">
-        <v>261</v>
-      </c>
-      <c r="H81" s="154" t="s">
-        <v>262</v>
-      </c>
-      <c r="I81" s="154" t="s">
-        <v>263</v>
-      </c>
-      <c r="J81" s="154" t="s">
-        <v>264</v>
-      </c>
-      <c r="K81" s="153"/>
-      <c r="L81" s="153"/>
-      <c r="M81" s="150"/>
-      <c r="N81" s="150"/>
-      <c r="O81" s="150"/>
-    </row>
-    <row r="82" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="155" t="s">
-        <v>265</v>
-      </c>
-      <c r="B82" s="155"/>
-      <c r="C82" s="155"/>
-      <c r="D82" s="155"/>
-      <c r="E82" s="156"/>
-      <c r="F82" s="155"/>
-      <c r="G82" s="155"/>
-      <c r="H82" s="157"/>
-      <c r="I82" s="155"/>
-      <c r="J82" s="155"/>
-      <c r="K82" s="155"/>
-      <c r="L82" s="155"/>
-      <c r="M82" s="155"/>
-      <c r="N82" s="155"/>
-      <c r="O82" s="155"/>
+      <c r="J86" s="130" t="s">
+        <v>278</v>
+      </c>
+      <c r="K86" s="154"/>
+      <c r="L86" s="154"/>
+      <c r="M86" s="151"/>
+      <c r="N86" s="151"/>
+      <c r="O86" s="151"/>
+    </row>
+    <row r="87" spans="1:15" s="9" customFormat="1">
+      <c r="A87" s="151"/>
+      <c r="B87" s="151"/>
+      <c r="C87" s="151"/>
+      <c r="D87" s="163"/>
+      <c r="E87" s="92"/>
+      <c r="F87" s="152" t="s">
+        <v>279</v>
+      </c>
+      <c r="G87" s="153" t="s">
+        <v>280</v>
+      </c>
+      <c r="H87" s="155" t="s">
+        <v>281</v>
+      </c>
+      <c r="I87" s="155" t="s">
+        <v>282</v>
+      </c>
+      <c r="J87" s="155" t="s">
+        <v>283</v>
+      </c>
+      <c r="K87" s="154"/>
+      <c r="L87" s="154"/>
+      <c r="M87" s="151"/>
+      <c r="N87" s="151"/>
+      <c r="O87" s="151"/>
+    </row>
+    <row r="88" spans="1:15" s="7" customFormat="1">
+      <c r="A88" s="156" t="s">
+        <v>284</v>
+      </c>
+      <c r="B88" s="156"/>
+      <c r="C88" s="156"/>
+      <c r="D88" s="156"/>
+      <c r="E88" s="157"/>
+      <c r="F88" s="156"/>
+      <c r="G88" s="156"/>
+      <c r="H88" s="158"/>
+      <c r="I88" s="156"/>
+      <c r="J88" s="156"/>
+      <c r="K88" s="156"/>
+      <c r="L88" s="156"/>
+      <c r="M88" s="156"/>
+      <c r="N88" s="156"/>
+      <c r="O88" s="156"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:O82" xr:uid="{FC96D3DE-56F6-4E60-B012-339ED5333B2B}">
+  <autoFilter ref="A9:O88" xr:uid="{FC96D3DE-56F6-4E60-B012-339ED5333B2B}">
     <filterColumn colId="0" showButton="0"/>
   </autoFilter>
   <mergeCells count="14">
+    <mergeCell ref="J2:O4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D18:D25"/>
     <mergeCell ref="D41:D63"/>
-    <mergeCell ref="D64:D81"/>
+    <mergeCell ref="D64:D87"/>
     <mergeCell ref="D27:D33"/>
     <mergeCell ref="D34:D40"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="D11:D15"/>
-    <mergeCell ref="J2:O4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D27">
@@ -4666,7 +4880,7 @@
       <formula>AND(NOT(ISBLANK($W41)),ISBLANK($AC41),ISBLANK($AD41))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F64:F67 G67:G79">
+  <conditionalFormatting sqref="F64:F67 G67:G85">
     <cfRule type="expression" dxfId="11" priority="117">
       <formula>AND($AD64=1,$AC64=1)</formula>
     </cfRule>
@@ -4707,13 +4921,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A95:A349" xr:uid="{F02B2F4C-E685-4FCA-8AD1-5712751D5727}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A101:A355" xr:uid="{F02B2F4C-E685-4FCA-8AD1-5712751D5727}">
       <formula1>"Envoi,Réception"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B23 C11:C23 B24:C347" xr:uid="{8AC62251-BDC4-4625-9564-FBEF29BC725C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:C353 B10:B23 C11:C23" xr:uid="{8AC62251-BDC4-4625-9564-FBEF29BC725C}">
       <formula1>"RC-EDA,RS-EDA,EMSI,EMSI-DC,EMSI-RDC,EMSI-EO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:A94" xr:uid="{22861EF6-4B68-4661-88F5-5CBBDF015C50}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:A100" xr:uid="{22861EF6-4B68-4661-88F5-5CBBDF015C50}">
       <formula1>"Envoi,Réception,End"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4724,55 +4938,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5190,50 +5361,65 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33493A62-AC11-48A7-B6C8-0591C55C368B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381C76DC-CEF1-461E-A76F-551B50E93033}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AEC75D3-A67D-4574-BB93-839AC9299105}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AEC75D3-A67D-4574-BB93-839AC9299105}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381C76DC-CEF1-461E-A76F-551B50E93033}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33493A62-AC11-48A7-B6C8-0591C55C368B}"/>
 </file>
</xml_diff>

<commit_message>
feat/test-cases: modify reception step json generation to generate one per dataset
</commit_message>
<xml_diff>
--- a/csv_parser/test-cases-15-15.xlsx
+++ b/csv_parser/test-cases-15-15.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/13 - 15-15/04 - Pilotes 15-15/04 - JDD recette/JSON pour interface LRM/03 - Automodel tracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ans-repos\SAMU-Hub-Modeles\csv_parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE9CDEF5-7CDC-46F5-B434-661C7097DB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D49C19B-6118-4E34-9AF5-612BBDB33072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="1590" windowWidth="22740" windowHeight="12930" xr2:uid="{8E95E427-60E8-4C01-A0F5-EF6B52DBDF48}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{8E95E427-60E8-4C01-A0F5-EF6B52DBDF48}"/>
   </bookViews>
   <sheets>
     <sheet name="Partage de dossier simple" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,9 @@
   <commentList>
     <comment ref="F65" authorId="0" shapeId="0" xr:uid="{FB75C0C9-7A43-4C0C-BF65-EEEEE383A568}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
     Pour savoir quelle alerte utiliser dans une affaire :
 =&gt; Regarder cette date de réception</t>
       </text>
@@ -567,9 +567,6 @@
     <t>Digicode 01</t>
   </si>
   <si>
-    <t>$.createCaseHealth.location.access[0].accessCode</t>
-  </si>
-  <si>
     <t>Ascenseur/escalier</t>
   </si>
   <si>
@@ -913,13 +910,16 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>$.createCaseHealth.location.access.accessCode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1926,9 +1926,21 @@
     <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1958,18 +1970,6 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2233,9 +2233,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2273,7 +2273,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2379,7 +2379,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2521,7 +2521,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2541,13 +2541,13 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="10" topLeftCell="G73" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G78" sqref="G78"/>
+      <pane xSplit="6" ySplit="10" topLeftCell="G46" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -2562,11 +2562,11 @@
     <col min="12" max="12" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75">
-      <c r="A1" s="159" t="s">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="159"/>
+      <c r="B1" s="160"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2583,11 +2583,11 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="18.75">
-      <c r="A2" s="159" t="s">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="160" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="159"/>
+      <c r="B2" s="160"/>
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
@@ -2599,20 +2599,20 @@
       <c r="I2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="170" t="s">
+      <c r="J2" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="18.75">
-      <c r="A3" s="159" t="s">
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="159"/>
+      <c r="B3" s="160"/>
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
@@ -2622,18 +2622,18 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170"/>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="18.75">
-      <c r="A4" s="159" t="s">
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
+      <c r="L3" s="159"/>
+      <c r="M3" s="159"/>
+      <c r="N3" s="159"/>
+      <c r="O3" s="159"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="159"/>
+      <c r="B4" s="160"/>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
@@ -2643,22 +2643,22 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
       <c r="I4" s="23"/>
-      <c r="J4" s="170"/>
-      <c r="K4" s="170"/>
-      <c r="L4" s="170"/>
-      <c r="M4" s="170"/>
-      <c r="N4" s="170"/>
-      <c r="O4" s="170"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="18.75">
-      <c r="A5" s="167" t="s">
+      <c r="J4" s="159"/>
+      <c r="K4" s="159"/>
+      <c r="L4" s="159"/>
+      <c r="M4" s="159"/>
+      <c r="N4" s="159"/>
+      <c r="O4" s="159"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="167"/>
-      <c r="C5" s="167"/>
-      <c r="D5" s="167"/>
-      <c r="E5" s="167"/>
-      <c r="F5" s="167"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
       <c r="I5" s="23"/>
@@ -2669,13 +2669,13 @@
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="18.75">
-      <c r="A6" s="171" t="s">
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="172"/>
-      <c r="C6" s="172"/>
-      <c r="D6" s="173"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="163"/>
       <c r="E6" s="21"/>
       <c r="F6" s="6" t="s">
         <v>11</v>
@@ -2690,13 +2690,13 @@
       <c r="N6" s="26"/>
       <c r="O6" s="26"/>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="18.75">
-      <c r="A7" s="168" t="s">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="172" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="168"/>
-      <c r="C7" s="168"/>
-      <c r="D7" s="168"/>
+      <c r="B7" s="172"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
       <c r="E7" s="27"/>
       <c r="F7" s="6" t="s">
         <v>13</v>
@@ -2711,7 +2711,7 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="18.75">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -2730,7 +2730,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
     </row>
-    <row r="9" spans="1:15" s="2" customFormat="1" ht="18.75">
+    <row r="9" spans="1:15" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>15</v>
       </c>
@@ -2771,7 +2771,7 @@
       <c r="N9" s="36"/>
       <c r="O9" s="36"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>26</v>
       </c>
@@ -2796,11 +2796,11 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:15" ht="16.5" customHeight="1">
+    <row r="11" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="169" t="s">
+      <c r="D11" s="173" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="42"/>
@@ -2825,11 +2825,11 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="169"/>
+      <c r="D12" s="173"/>
       <c r="E12" s="42"/>
       <c r="F12" s="47" t="s">
         <v>36</v>
@@ -2852,11 +2852,11 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="169"/>
+      <c r="D13" s="173"/>
       <c r="E13" s="42"/>
       <c r="F13" s="51" t="s">
         <v>39</v>
@@ -2879,11 +2879,11 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15" s="4" customFormat="1">
+    <row r="14" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="52"/>
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
-      <c r="D14" s="169"/>
+      <c r="D14" s="173"/>
       <c r="E14" s="17">
         <v>3</v>
       </c>
@@ -2908,11 +2908,11 @@
       <c r="N14" s="52"/>
       <c r="O14" s="52"/>
     </row>
-    <row r="15" spans="1:15" s="4" customFormat="1">
+    <row r="15" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
-      <c r="D15" s="169"/>
+      <c r="D15" s="173"/>
       <c r="E15" s="17">
         <v>3</v>
       </c>
@@ -2937,7 +2937,7 @@
       <c r="N15" s="52"/>
       <c r="O15" s="52"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2960,7 +2960,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2983,11 +2983,11 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="160" t="s">
+      <c r="D18" s="164" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="42">
@@ -3014,11 +3014,11 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" ht="28.5" customHeight="1">
+    <row r="19" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="161"/>
+      <c r="D19" s="165"/>
       <c r="E19" s="42">
         <v>3</v>
       </c>
@@ -3043,11 +3043,11 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="161"/>
+      <c r="D20" s="165"/>
       <c r="E20" s="17">
         <v>2</v>
       </c>
@@ -3072,11 +3072,11 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15" s="8" customFormat="1" ht="30.75">
+    <row r="21" spans="1:15" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="75"/>
       <c r="B21" s="75"/>
       <c r="C21" s="75"/>
-      <c r="D21" s="161"/>
+      <c r="D21" s="165"/>
       <c r="E21" s="76">
         <v>3</v>
       </c>
@@ -3101,11 +3101,11 @@
       <c r="N21" s="75"/>
       <c r="O21" s="75"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="161"/>
+      <c r="D22" s="165"/>
       <c r="E22" s="17">
         <v>1</v>
       </c>
@@ -3130,11 +3130,11 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
     </row>
-    <row r="23" spans="1:15" ht="30.75" customHeight="1">
+    <row r="23" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="161"/>
+      <c r="D23" s="165"/>
       <c r="E23" s="76">
         <v>3</v>
       </c>
@@ -3159,11 +3159,11 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="161"/>
+      <c r="D24" s="165"/>
       <c r="E24" s="17">
         <v>1</v>
       </c>
@@ -3188,11 +3188,11 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="162"/>
+      <c r="D25" s="166"/>
       <c r="E25" s="85">
         <v>3</v>
       </c>
@@ -3217,7 +3217,7 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -3248,11 +3248,11 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="164" t="s">
+      <c r="D27" s="168" t="s">
         <v>98</v>
       </c>
       <c r="E27" s="92"/>
@@ -3277,11 +3277,11 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="165"/>
+      <c r="D28" s="169"/>
       <c r="E28" s="17">
         <v>1</v>
       </c>
@@ -3306,8 +3306,8 @@
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:15" s="6" customFormat="1">
-      <c r="D29" s="165"/>
+    <row r="29" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="169"/>
       <c r="E29" s="17">
         <v>2</v>
       </c>
@@ -3327,11 +3327,11 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="165"/>
+      <c r="D30" s="169"/>
       <c r="E30" s="17">
         <v>1</v>
       </c>
@@ -3354,11 +3354,11 @@
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="165"/>
+      <c r="D31" s="169"/>
       <c r="E31" s="17"/>
       <c r="F31" s="13" t="s">
         <v>117</v>
@@ -3379,11 +3379,11 @@
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="165"/>
+      <c r="D32" s="169"/>
       <c r="E32" s="17"/>
       <c r="F32" s="13" t="s">
         <v>121</v>
@@ -3404,11 +3404,11 @@
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
     </row>
-    <row r="33" spans="1:15" s="4" customFormat="1">
+    <row r="33" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="52"/>
       <c r="B33" s="52"/>
       <c r="C33" s="52"/>
-      <c r="D33" s="165"/>
+      <c r="D33" s="169"/>
       <c r="E33" s="17">
         <v>2</v>
       </c>
@@ -3433,11 +3433,11 @@
       <c r="N33" s="52"/>
       <c r="O33" s="52"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="164" t="s">
+      <c r="D34" s="168" t="s">
         <v>130</v>
       </c>
       <c r="E34" s="92"/>
@@ -3456,11 +3456,11 @@
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="165"/>
+      <c r="D35" s="169"/>
       <c r="E35" s="17"/>
       <c r="F35" s="13" t="s">
         <v>104</v>
@@ -3477,11 +3477,11 @@
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="165"/>
+      <c r="D36" s="169"/>
       <c r="E36" s="17"/>
       <c r="F36" s="13" t="s">
         <v>109</v>
@@ -3498,11 +3498,11 @@
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="165"/>
+      <c r="D37" s="169"/>
       <c r="E37" s="17"/>
       <c r="F37" s="13" t="s">
         <v>113</v>
@@ -3519,11 +3519,11 @@
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="165"/>
+      <c r="D38" s="169"/>
       <c r="E38" s="17"/>
       <c r="F38" s="13" t="s">
         <v>117</v>
@@ -3540,11 +3540,11 @@
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="165"/>
+      <c r="D39" s="169"/>
       <c r="E39" s="17"/>
       <c r="F39" s="13" t="s">
         <v>121</v>
@@ -3561,11 +3561,11 @@
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
-      <c r="D40" s="166"/>
+      <c r="D40" s="170"/>
       <c r="E40" s="17"/>
       <c r="F40" s="105" t="s">
         <v>125</v>
@@ -3582,11 +3582,11 @@
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="160" t="s">
+      <c r="D41" s="164" t="s">
         <v>138</v>
       </c>
       <c r="E41" s="42"/>
@@ -3611,11 +3611,11 @@
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
-      <c r="D42" s="161"/>
+      <c r="D42" s="165"/>
       <c r="E42" s="17">
         <v>2</v>
       </c>
@@ -3640,11 +3640,11 @@
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
     </row>
-    <row r="43" spans="1:15" s="4" customFormat="1">
+    <row r="43" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="52"/>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>
-      <c r="D43" s="161"/>
+      <c r="D43" s="165"/>
       <c r="E43" s="17"/>
       <c r="F43" s="114" t="s">
         <v>147</v>
@@ -3663,11 +3663,11 @@
       <c r="N43" s="52"/>
       <c r="O43" s="52"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="161"/>
+      <c r="D44" s="165"/>
       <c r="E44" s="92">
         <v>1</v>
       </c>
@@ -3692,11 +3692,11 @@
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
-      <c r="D45" s="161"/>
+      <c r="D45" s="165"/>
       <c r="E45" s="17">
         <v>1</v>
       </c>
@@ -3721,11 +3721,11 @@
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="161"/>
+      <c r="D46" s="165"/>
       <c r="E46" s="17">
         <v>3</v>
       </c>
@@ -3750,11 +3750,11 @@
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
-      <c r="D47" s="161"/>
+      <c r="D47" s="165"/>
       <c r="E47" s="17">
         <v>2</v>
       </c>
@@ -3775,11 +3775,11 @@
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
-      <c r="D48" s="161"/>
+      <c r="D48" s="165"/>
       <c r="E48" s="17">
         <v>2</v>
       </c>
@@ -3798,11 +3798,11 @@
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="161"/>
+      <c r="D49" s="165"/>
       <c r="E49" s="17">
         <v>2</v>
       </c>
@@ -3823,11 +3823,11 @@
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
-      <c r="D50" s="161"/>
+      <c r="D50" s="165"/>
       <c r="E50" s="17">
         <v>2</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>168</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>169</v>
+        <v>284</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="123">
@@ -3848,23 +3848,23 @@
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
-      <c r="D51" s="161"/>
+      <c r="D51" s="165"/>
       <c r="E51" s="17">
         <v>2</v>
       </c>
       <c r="F51" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
@@ -3873,23 +3873,23 @@
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
-      <c r="D52" s="161"/>
+      <c r="D52" s="165"/>
       <c r="E52" s="17">
         <v>2</v>
       </c>
       <c r="F52" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
@@ -3898,19 +3898,19 @@
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
-      <c r="D53" s="161"/>
+      <c r="D53" s="165"/>
       <c r="E53" s="17">
         <v>2</v>
       </c>
       <c r="F53" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
@@ -3921,19 +3921,19 @@
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
-      <c r="D54" s="161"/>
+      <c r="D54" s="165"/>
       <c r="E54" s="17">
         <v>2</v>
       </c>
       <c r="F54" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -3944,19 +3944,19 @@
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
-      <c r="D55" s="161"/>
+      <c r="D55" s="165"/>
       <c r="E55" s="17">
         <v>2</v>
       </c>
       <c r="F55" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>181</v>
       </c>
       <c r="H55" s="125"/>
       <c r="I55" s="125"/>
@@ -3969,28 +3969,28 @@
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
     </row>
-    <row r="56" spans="1:15" s="4" customFormat="1">
+    <row r="56" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="52"/>
       <c r="B56" s="52"/>
       <c r="C56" s="52"/>
-      <c r="D56" s="161"/>
+      <c r="D56" s="165"/>
       <c r="E56" s="17">
         <v>2</v>
       </c>
       <c r="F56" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="H56" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="H56" s="54" t="s">
+      <c r="I56" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="I56" s="54" t="s">
+      <c r="J56" s="126" t="s">
         <v>185</v>
-      </c>
-      <c r="J56" s="126" t="s">
-        <v>186</v>
       </c>
       <c r="K56" s="97"/>
       <c r="L56" s="97"/>
@@ -3998,23 +3998,23 @@
       <c r="N56" s="52"/>
       <c r="O56" s="52"/>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
-      <c r="D57" s="161"/>
+      <c r="D57" s="165"/>
       <c r="E57" s="92"/>
       <c r="F57" s="127" t="s">
+        <v>186</v>
+      </c>
+      <c r="G57" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="G57" s="128" t="s">
+      <c r="H57" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="H57" s="128" t="s">
-        <v>189</v>
-      </c>
       <c r="I57" s="129" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J57" s="128"/>
       <c r="K57" s="81"/>
@@ -4023,25 +4023,25 @@
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="161"/>
+      <c r="D58" s="165"/>
       <c r="E58" s="92">
         <v>3</v>
       </c>
       <c r="F58" s="130" t="s">
+        <v>189</v>
+      </c>
+      <c r="G58" s="128" t="s">
         <v>190</v>
       </c>
-      <c r="G58" s="128" t="s">
+      <c r="H58" s="131" t="s">
         <v>191</v>
       </c>
-      <c r="H58" s="131" t="s">
+      <c r="I58" s="132" t="s">
         <v>192</v>
-      </c>
-      <c r="I58" s="132" t="s">
-        <v>193</v>
       </c>
       <c r="J58" s="131"/>
       <c r="K58" s="81"/>
@@ -4050,25 +4050,25 @@
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
-      <c r="D59" s="161"/>
+      <c r="D59" s="165"/>
       <c r="E59" s="92">
         <v>3</v>
       </c>
       <c r="F59" s="130" t="s">
+        <v>193</v>
+      </c>
+      <c r="G59" s="128" t="s">
         <v>194</v>
       </c>
-      <c r="G59" s="128" t="s">
+      <c r="H59" s="131" t="s">
         <v>195</v>
       </c>
-      <c r="H59" s="131" t="s">
+      <c r="I59" s="132" t="s">
         <v>196</v>
-      </c>
-      <c r="I59" s="132" t="s">
-        <v>197</v>
       </c>
       <c r="J59" s="131"/>
       <c r="K59" s="81"/>
@@ -4077,17 +4077,17 @@
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
-      <c r="D60" s="161"/>
+      <c r="D60" s="165"/>
       <c r="E60" s="17"/>
       <c r="F60" s="133" t="s">
+        <v>197</v>
+      </c>
+      <c r="G60" s="120" t="s">
         <v>198</v>
-      </c>
-      <c r="G60" s="120" t="s">
-        <v>199</v>
       </c>
       <c r="H60" s="120"/>
       <c r="I60" s="5"/>
@@ -4098,17 +4098,17 @@
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
-      <c r="D61" s="161"/>
+      <c r="D61" s="165"/>
       <c r="E61" s="17"/>
       <c r="F61" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="G61" s="120" t="s">
         <v>200</v>
-      </c>
-      <c r="G61" s="120" t="s">
-        <v>201</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
@@ -4119,17 +4119,17 @@
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
-      <c r="D62" s="161"/>
+      <c r="D62" s="165"/>
       <c r="E62" s="17"/>
       <c r="F62" s="124" t="s">
+        <v>201</v>
+      </c>
+      <c r="G62" s="120" t="s">
         <v>202</v>
-      </c>
-      <c r="G62" s="120" t="s">
-        <v>203</v>
       </c>
       <c r="H62" s="125"/>
       <c r="I62" s="5"/>
@@ -4140,23 +4140,23 @@
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
-      <c r="D63" s="162"/>
+      <c r="D63" s="166"/>
       <c r="E63" s="92"/>
       <c r="F63" s="130" t="s">
+        <v>203</v>
+      </c>
+      <c r="G63" s="128" t="s">
         <v>204</v>
       </c>
-      <c r="G63" s="128" t="s">
+      <c r="H63" s="134" t="s">
         <v>205</v>
       </c>
-      <c r="H63" s="134" t="s">
-        <v>206</v>
-      </c>
       <c r="I63" s="134" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J63" s="134"/>
       <c r="K63" s="81"/>
@@ -4165,28 +4165,28 @@
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
-      <c r="D64" s="163" t="s">
-        <v>207</v>
+      <c r="D64" s="167" t="s">
+        <v>206</v>
       </c>
       <c r="E64" s="92"/>
       <c r="F64" s="135" t="s">
+        <v>207</v>
+      </c>
+      <c r="G64" s="128" t="s">
         <v>208</v>
       </c>
-      <c r="G64" s="128" t="s">
+      <c r="H64" s="134" t="s">
         <v>209</v>
       </c>
-      <c r="H64" s="134" t="s">
+      <c r="I64" s="134" t="s">
         <v>210</v>
       </c>
-      <c r="I64" s="134" t="s">
+      <c r="J64" s="134" t="s">
         <v>211</v>
-      </c>
-      <c r="J64" s="134" t="s">
-        <v>212</v>
       </c>
       <c r="K64" s="81"/>
       <c r="L64" s="81"/>
@@ -4194,17 +4194,17 @@
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
-      <c r="D65" s="163"/>
+      <c r="D65" s="167"/>
       <c r="E65" s="92"/>
       <c r="F65" s="136" t="s">
+        <v>212</v>
+      </c>
+      <c r="G65" s="128" t="s">
         <v>213</v>
-      </c>
-      <c r="G65" s="128" t="s">
-        <v>214</v>
       </c>
       <c r="H65" s="137" t="s">
         <v>38</v>
@@ -4221,26 +4221,26 @@
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
-      <c r="D66" s="163"/>
+      <c r="D66" s="167"/>
       <c r="E66" s="17"/>
       <c r="F66" s="136" t="s">
+        <v>214</v>
+      </c>
+      <c r="G66" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="G66" s="128" t="s">
+      <c r="H66" s="137" t="s">
         <v>216</v>
       </c>
-      <c r="H66" s="137" t="s">
-        <v>217</v>
-      </c>
       <c r="I66" s="137" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J66" s="137" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K66" s="81"/>
       <c r="L66" s="81"/>
@@ -4248,19 +4248,19 @@
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1">
+    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
-      <c r="D67" s="163"/>
+      <c r="D67" s="167"/>
       <c r="E67" s="17">
         <v>2</v>
       </c>
       <c r="F67" s="138" t="s">
+        <v>217</v>
+      </c>
+      <c r="G67" s="139" t="s">
         <v>218</v>
-      </c>
-      <c r="G67" s="139" t="s">
-        <v>219</v>
       </c>
       <c r="H67" s="140"/>
       <c r="I67" s="140"/>
@@ -4271,28 +4271,28 @@
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
-      <c r="D68" s="163"/>
+      <c r="D68" s="167"/>
       <c r="E68" s="17">
         <v>1</v>
       </c>
       <c r="F68" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="G68" s="139" t="s">
         <v>220</v>
       </c>
-      <c r="G68" s="139" t="s">
+      <c r="H68" s="60" t="s">
         <v>221</v>
       </c>
-      <c r="H68" s="60" t="s">
-        <v>222</v>
-      </c>
       <c r="I68" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J68" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K68" s="13"/>
       <c r="L68" s="5"/>
@@ -4300,19 +4300,19 @@
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
     </row>
-    <row r="69" spans="1:15" s="6" customFormat="1">
-      <c r="D69" s="163"/>
+    <row r="69" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="167"/>
       <c r="E69" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F69" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="F69" s="19" t="s">
+      <c r="G69" s="139" t="s">
         <v>224</v>
       </c>
-      <c r="G69" s="139" t="s">
+      <c r="H69" s="16" t="s">
         <v>225</v>
-      </c>
-      <c r="H69" s="16" t="s">
-        <v>226</v>
       </c>
       <c r="I69" s="16">
         <v>702880946</v>
@@ -4323,49 +4323,49 @@
       <c r="K69" s="13"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:15" s="10" customFormat="1">
-      <c r="D70" s="163"/>
+    <row r="70" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D70" s="167"/>
       <c r="E70" s="18"/>
       <c r="F70" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="G70" s="141" t="s">
         <v>227</v>
       </c>
-      <c r="G70" s="141" t="s">
+      <c r="H70" s="142" t="s">
         <v>228</v>
       </c>
-      <c r="H70" s="142" t="s">
-        <v>229</v>
-      </c>
       <c r="I70" s="142" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J70" s="142" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K70" s="14"/>
       <c r="L70" s="11"/>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
-      <c r="D71" s="163"/>
+      <c r="D71" s="167"/>
       <c r="E71" s="17">
         <v>2</v>
       </c>
       <c r="F71" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="G71" s="139" t="s">
         <v>230</v>
       </c>
-      <c r="G71" s="139" t="s">
-        <v>231</v>
-      </c>
       <c r="H71" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I71" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J71" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K71" s="13"/>
       <c r="L71" s="5"/>
@@ -4373,19 +4373,19 @@
       <c r="N71" s="6"/>
       <c r="O71" s="6"/>
     </row>
-    <row r="72" spans="1:15" s="6" customFormat="1">
-      <c r="D72" s="163"/>
+    <row r="72" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D72" s="167"/>
       <c r="E72" s="17">
         <v>2</v>
       </c>
       <c r="F72" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="G72" s="139" t="s">
         <v>232</v>
       </c>
-      <c r="G72" s="139" t="s">
-        <v>233</v>
-      </c>
       <c r="H72" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I72" s="16">
         <v>702880946</v>
@@ -4396,35 +4396,35 @@
       <c r="K72" s="13"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:15" s="10" customFormat="1">
-      <c r="D73" s="163"/>
+    <row r="73" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D73" s="167"/>
       <c r="E73" s="18"/>
       <c r="F73" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="G73" s="141" t="s">
         <v>234</v>
       </c>
-      <c r="G73" s="141" t="s">
-        <v>235</v>
-      </c>
       <c r="H73" s="142" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I73" s="142" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J73" s="142" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K73" s="14"/>
       <c r="L73" s="11"/>
     </row>
-    <row r="74" spans="1:15" s="6" customFormat="1">
-      <c r="D74" s="163"/>
+    <row r="74" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D74" s="167"/>
       <c r="E74" s="17"/>
       <c r="F74" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="G74" s="139" t="s">
         <v>236</v>
-      </c>
-      <c r="G74" s="139" t="s">
-        <v>237</v>
       </c>
       <c r="H74" s="15" t="s">
         <v>146</v>
@@ -4438,28 +4438,28 @@
       <c r="K74" s="13"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
-      <c r="D75" s="163"/>
+      <c r="D75" s="167"/>
       <c r="E75" s="17">
         <v>3</v>
       </c>
       <c r="F75" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="G75" s="139" t="s">
         <v>238</v>
       </c>
-      <c r="G75" s="139" t="s">
+      <c r="H75" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="H75" s="143" t="s">
+      <c r="I75" s="61" t="s">
         <v>240</v>
       </c>
-      <c r="I75" s="61" t="s">
-        <v>241</v>
-      </c>
       <c r="J75" s="61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K75" s="13"/>
       <c r="L75" s="5"/>
@@ -4467,17 +4467,17 @@
       <c r="N75" s="6"/>
       <c r="O75" s="6"/>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
-      <c r="D76" s="163"/>
+      <c r="D76" s="167"/>
       <c r="E76" s="17"/>
       <c r="F76" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="G76" s="139" t="s">
         <v>242</v>
-      </c>
-      <c r="G76" s="139" t="s">
-        <v>243</v>
       </c>
       <c r="H76" s="143"/>
       <c r="I76" s="61"/>
@@ -4488,17 +4488,17 @@
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
-      <c r="D77" s="163"/>
+      <c r="D77" s="167"/>
       <c r="E77" s="17"/>
       <c r="F77" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="G77" s="139" t="s">
         <v>244</v>
-      </c>
-      <c r="G77" s="139" t="s">
-        <v>245</v>
       </c>
       <c r="H77" s="60"/>
       <c r="I77" s="61"/>
@@ -4509,28 +4509,28 @@
       <c r="N77" s="6"/>
       <c r="O77" s="6"/>
     </row>
-    <row r="78" spans="1:15" ht="30.75">
+    <row r="78" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
-      <c r="D78" s="163"/>
+      <c r="D78" s="167"/>
       <c r="E78" s="17">
         <v>2</v>
       </c>
       <c r="F78" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="G78" s="139" t="s">
         <v>246</v>
       </c>
-      <c r="G78" s="139" t="s">
+      <c r="H78" s="144" t="s">
         <v>247</v>
       </c>
-      <c r="H78" s="144" t="s">
+      <c r="I78" s="144" t="s">
         <v>248</v>
       </c>
-      <c r="I78" s="144" t="s">
+      <c r="J78" s="144" t="s">
         <v>249</v>
-      </c>
-      <c r="J78" s="144" t="s">
-        <v>250</v>
       </c>
       <c r="K78" s="61"/>
       <c r="L78" s="13"/>
@@ -4538,17 +4538,17 @@
       <c r="N78" s="6"/>
       <c r="O78" s="6"/>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
-      <c r="D79" s="163"/>
+      <c r="D79" s="167"/>
       <c r="E79" s="17"/>
       <c r="F79" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="G79" s="139" t="s">
         <v>251</v>
-      </c>
-      <c r="G79" s="139" t="s">
-        <v>252</v>
       </c>
       <c r="H79" s="22"/>
       <c r="I79" s="6"/>
@@ -4559,25 +4559,25 @@
       <c r="N79" s="6"/>
       <c r="O79" s="6"/>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
-      <c r="D80" s="163"/>
+      <c r="D80" s="167"/>
       <c r="E80" s="17">
         <v>2</v>
       </c>
       <c r="F80" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="G80" s="139" t="s">
         <v>253</v>
       </c>
-      <c r="G80" s="139" t="s">
+      <c r="H80" s="60" t="s">
         <v>254</v>
       </c>
-      <c r="H80" s="60" t="s">
+      <c r="I80" s="61" t="s">
         <v>255</v>
-      </c>
-      <c r="I80" s="61" t="s">
-        <v>256</v>
       </c>
       <c r="J80" s="19"/>
       <c r="K80" s="61"/>
@@ -4586,17 +4586,17 @@
       <c r="N80" s="6"/>
       <c r="O80" s="6"/>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
-      <c r="D81" s="163"/>
+      <c r="D81" s="167"/>
       <c r="E81" s="17"/>
       <c r="F81" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="G81" s="139" t="s">
         <v>257</v>
-      </c>
-      <c r="G81" s="139" t="s">
-        <v>258</v>
       </c>
       <c r="H81" s="60"/>
       <c r="I81" s="61"/>
@@ -4607,23 +4607,23 @@
       <c r="N81" s="6"/>
       <c r="O81" s="6"/>
     </row>
-    <row r="82" spans="1:15" ht="14.25" customHeight="1">
+    <row r="82" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
-      <c r="D82" s="163"/>
+      <c r="D82" s="167"/>
       <c r="E82" s="17">
         <v>2</v>
       </c>
       <c r="F82" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="G82" s="139" t="s">
         <v>259</v>
-      </c>
-      <c r="G82" s="139" t="s">
-        <v>260</v>
       </c>
       <c r="H82" s="60"/>
       <c r="I82" s="61" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J82" s="133"/>
       <c r="K82" s="120"/>
@@ -4632,28 +4632,28 @@
       <c r="N82" s="6"/>
       <c r="O82" s="6"/>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
-      <c r="D83" s="163"/>
+      <c r="D83" s="167"/>
       <c r="E83" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F83" s="145" t="s">
+        <v>261</v>
+      </c>
+      <c r="G83" s="139" t="s">
         <v>262</v>
       </c>
-      <c r="G83" s="139" t="s">
+      <c r="H83" s="146" t="s">
         <v>263</v>
       </c>
-      <c r="H83" s="146" t="s">
+      <c r="I83" s="146" t="s">
         <v>264</v>
       </c>
-      <c r="I83" s="146" t="s">
+      <c r="J83" s="93" t="s">
         <v>265</v>
-      </c>
-      <c r="J83" s="93" t="s">
-        <v>266</v>
       </c>
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
@@ -4661,26 +4661,26 @@
       <c r="N83" s="6"/>
       <c r="O83" s="6"/>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
-      <c r="D84" s="163"/>
+      <c r="D84" s="167"/>
       <c r="E84" s="17"/>
       <c r="F84" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="G84" s="139" t="s">
         <v>267</v>
       </c>
-      <c r="G84" s="139" t="s">
+      <c r="H84" s="60" t="s">
         <v>268</v>
       </c>
-      <c r="H84" s="60" t="s">
+      <c r="I84" s="61" t="s">
         <v>269</v>
       </c>
-      <c r="I84" s="61" t="s">
+      <c r="J84" s="13" t="s">
         <v>270</v>
-      </c>
-      <c r="J84" s="13" t="s">
-        <v>271</v>
       </c>
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
@@ -4688,26 +4688,26 @@
       <c r="N84" s="6"/>
       <c r="O84" s="6"/>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
-      <c r="D85" s="163"/>
+      <c r="D85" s="167"/>
       <c r="E85" s="17"/>
       <c r="F85" s="147" t="s">
+        <v>271</v>
+      </c>
+      <c r="G85" s="148" t="s">
         <v>272</v>
-      </c>
-      <c r="G85" s="148" t="s">
-        <v>273</v>
       </c>
       <c r="H85" s="149" t="s">
         <v>123</v>
       </c>
       <c r="I85" s="150" t="s">
+        <v>273</v>
+      </c>
+      <c r="J85" s="125" t="s">
         <v>274</v>
-      </c>
-      <c r="J85" s="125" t="s">
-        <v>275</v>
       </c>
       <c r="K85" s="125"/>
       <c r="L85" s="125"/>
@@ -4715,17 +4715,17 @@
       <c r="N85" s="6"/>
       <c r="O85" s="6"/>
     </row>
-    <row r="86" spans="1:15" s="9" customFormat="1">
+    <row r="86" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="151"/>
       <c r="B86" s="151"/>
       <c r="C86" s="151"/>
-      <c r="D86" s="163"/>
+      <c r="D86" s="167"/>
       <c r="E86" s="92"/>
       <c r="F86" s="152" t="s">
+        <v>275</v>
+      </c>
+      <c r="G86" s="153" t="s">
         <v>276</v>
-      </c>
-      <c r="G86" s="153" t="s">
-        <v>277</v>
       </c>
       <c r="H86" s="130" t="s">
         <v>95</v>
@@ -4734,7 +4734,7 @@
         <v>96</v>
       </c>
       <c r="J86" s="130" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K86" s="154"/>
       <c r="L86" s="154"/>
@@ -4742,26 +4742,26 @@
       <c r="N86" s="151"/>
       <c r="O86" s="151"/>
     </row>
-    <row r="87" spans="1:15" s="9" customFormat="1">
+    <row r="87" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="151"/>
       <c r="B87" s="151"/>
       <c r="C87" s="151"/>
-      <c r="D87" s="163"/>
+      <c r="D87" s="167"/>
       <c r="E87" s="92"/>
       <c r="F87" s="152" t="s">
+        <v>278</v>
+      </c>
+      <c r="G87" s="153" t="s">
         <v>279</v>
       </c>
-      <c r="G87" s="153" t="s">
+      <c r="H87" s="155" t="s">
         <v>280</v>
       </c>
-      <c r="H87" s="155" t="s">
+      <c r="I87" s="155" t="s">
         <v>281</v>
       </c>
-      <c r="I87" s="155" t="s">
+      <c r="J87" s="155" t="s">
         <v>282</v>
-      </c>
-      <c r="J87" s="155" t="s">
-        <v>283</v>
       </c>
       <c r="K87" s="154"/>
       <c r="L87" s="154"/>
@@ -4769,9 +4769,9 @@
       <c r="N87" s="151"/>
       <c r="O87" s="151"/>
     </row>
-    <row r="88" spans="1:15" s="7" customFormat="1">
+    <row r="88" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="156" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B88" s="156"/>
       <c r="C88" s="156"/>
@@ -4793,11 +4793,6 @@
     <filterColumn colId="0" showButton="0"/>
   </autoFilter>
   <mergeCells count="14">
-    <mergeCell ref="J2:O4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D18:D25"/>
     <mergeCell ref="D41:D63"/>
@@ -4807,6 +4802,11 @@
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="D11:D15"/>
+    <mergeCell ref="J2:O4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D27">
@@ -4938,15 +4938,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5360,6 +5351,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5413,13 +5413,41 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381C76DC-CEF1-461E-A76F-551B50E93033}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AEC75D3-A67D-4574-BB93-839AC9299105}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AEC75D3-A67D-4574-BB93-839AC9299105}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381C76DC-CEF1-461E-A76F-551B50E93033}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33493A62-AC11-48A7-B6C8-0591C55C368B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33493A62-AC11-48A7-B6C8-0591C55C368B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>